<commit_message>
Add FY17 & FY18 to £VOD model
</commit_message>
<xml_diff>
--- a/£VOD.xlsx
+++ b/£VOD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2549E51C-8D75-4F62-A4B9-9D061D218A3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65873D97-D29C-4D88-816B-06531D9366DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{5E4D6509-12BB-42E6-9952-4B32877F48D2}"/>
   </bookViews>
@@ -343,7 +343,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -602,15 +602,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -628,18 +619,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -668,12 +647,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -715,14 +688,41 @@
     <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1214,7 +1214,7 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="C28" sqref="C28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1234,593 +1234,588 @@
       <c r="F3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="G5" s="4" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="G5" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="55"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>1.0247999999999999</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="G6" s="29">
+      <c r="D6" s="7"/>
+      <c r="G6" s="22">
         <v>44835</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="13"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="15">
         <v>29012</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="7" t="str">
         <f>$C$27</f>
         <v>FY22</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="13"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="15">
         <f>C6*C7</f>
         <v>29731.497599999999</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="13"/>
+      <c r="D8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="15">
         <f>'Financial Model'!U72*Main!$C$13</f>
         <v>6596.4800000000005</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="7" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$27</f>
         <v>FY22</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="13"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="15">
         <f>'Financial Model'!U73*Main!$C$13</f>
         <v>62115.68</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FY22</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="13"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="15">
         <f>C9-C10</f>
         <v>-55519.199999999997</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>FY22</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="13"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="16">
         <f>C8-C11</f>
         <v>85250.6976</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="13"/>
+      <c r="D12" s="8"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="55">
+      <c r="C13" s="46">
         <v>0.88</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13"/>
+      <c r="D13" s="47"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G14" s="27"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="13"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="13"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="13"/>
+      <c r="D16" s="57"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="13"/>
+      <c r="D17" s="57"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="13"/>
+      <c r="D18" s="57"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="13"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G20" s="27"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="13"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G21" s="27"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="13"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="13"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="13"/>
+      <c r="D23" s="57"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="56">
         <v>1984</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="13"/>
+      <c r="D24" s="57"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="10"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="64">
+      <c r="C25" s="62">
         <f>'Financial Model'!U42</f>
         <v>836</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="13"/>
+      <c r="D25" s="57"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="16"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="51">
         <v>44621</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="13"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="13"/>
+      <c r="D28" s="59"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="10"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G29" s="27"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="13"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="10"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G30" s="27"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="13"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="13"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="10"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="61">
+      <c r="C32" s="60">
         <f>C6/'Financial Model'!U67</f>
         <v>0.52181577829650561</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="13"/>
+      <c r="D32" s="61"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="13"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="10"/>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="61">
+      <c r="C34" s="60">
         <f>C6/'Financial Model'!U20</f>
         <v>11.330601219512195</v>
       </c>
-      <c r="D34" s="62"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="15"/>
+      <c r="D34" s="61"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B5:D5"/>
@@ -1833,6 +1828,11 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{D050E430-21A3-4017-A567-1BB4BBA21237}"/>
@@ -1850,7 +1850,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T83" sqref="R83:T83"/>
+      <selection pane="bottomRight" activeCell="R83" sqref="P83:R85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1858,123 +1858,132 @@
     <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="9.140625" style="33"/>
+    <col min="4" max="4" width="9.140625" style="26"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="33"/>
+    <col min="6" max="6" width="9.140625" style="26"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="33"/>
+    <col min="8" max="8" width="9.140625" style="26"/>
     <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="33"/>
+    <col min="10" max="10" width="9.140625" style="26"/>
     <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="9.140625" style="33"/>
+    <col min="12" max="12" width="9.140625" style="26"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="31" t="s">
+      <c r="W1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="X1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Y1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="Z1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AA1" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:27" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36"/>
-      <c r="D2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="R2" s="40">
+    <row r="2" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="27"/>
+      <c r="D2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="P2" s="31">
+        <v>42825</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>43190</v>
+      </c>
+      <c r="R2" s="31">
         <v>43555</v>
       </c>
-      <c r="S2" s="40">
+      <c r="S2" s="31">
         <v>43921</v>
       </c>
-      <c r="T2" s="40">
+      <c r="T2" s="31">
         <v>44286</v>
       </c>
-      <c r="U2" s="40">
+      <c r="U2" s="31">
         <v>44651</v>
       </c>
     </row>
-    <row r="3" spans="2:27" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="36"/>
-      <c r="D3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="S3" s="39">
+    <row r="3" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="27"/>
+      <c r="D3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="Q3" s="30">
+        <v>43235</v>
+      </c>
+      <c r="S3" s="30">
         <v>43963</v>
       </c>
-      <c r="U3" s="39">
+      <c r="U3" s="30">
         <v>44708</v>
       </c>
     </row>
@@ -1982,21 +1991,27 @@
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="R4" s="43">
+      <c r="D4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="P4" s="34">
+        <v>47631</v>
+      </c>
+      <c r="Q4" s="34">
+        <v>46571</v>
+      </c>
+      <c r="R4" s="34">
         <v>43666</v>
       </c>
-      <c r="S4" s="43">
+      <c r="S4" s="34">
         <v>44974</v>
       </c>
-      <c r="T4" s="43">
+      <c r="T4" s="34">
         <v>43809</v>
       </c>
-      <c r="U4" s="43">
+      <c r="U4" s="34">
         <v>45580</v>
       </c>
     </row>
@@ -2004,16 +2019,22 @@
       <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R5" s="44">
+      <c r="P5" s="35">
+        <v>34576</v>
+      </c>
+      <c r="Q5" s="35">
+        <v>32771</v>
+      </c>
+      <c r="R5" s="35">
         <v>30160</v>
       </c>
-      <c r="S5" s="44">
+      <c r="S5" s="35">
         <v>30682</v>
       </c>
-      <c r="T5" s="44">
+      <c r="T5" s="35">
         <v>30086</v>
       </c>
-      <c r="U5" s="44">
+      <c r="U5" s="35">
         <v>30574</v>
       </c>
     </row>
@@ -2021,24 +2042,32 @@
       <c r="B6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="R6" s="43">
+      <c r="D6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="P6" s="34">
+        <f t="shared" ref="P6:Q6" si="0">P4-P5</f>
+        <v>13055</v>
+      </c>
+      <c r="Q6" s="34">
+        <f t="shared" si="0"/>
+        <v>13800</v>
+      </c>
+      <c r="R6" s="34">
         <f>R4-R5</f>
         <v>13506</v>
       </c>
-      <c r="S6" s="43">
+      <c r="S6" s="34">
         <f>S4-S5</f>
         <v>14292</v>
       </c>
-      <c r="T6" s="43">
+      <c r="T6" s="34">
         <f>T4-T5</f>
         <v>13723</v>
       </c>
-      <c r="U6" s="43">
+      <c r="U6" s="34">
         <f>U4-U5</f>
         <v>15006</v>
       </c>
@@ -2047,16 +2076,22 @@
       <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R7" s="44">
+      <c r="P7" s="35">
+        <v>4349</v>
+      </c>
+      <c r="Q7" s="35">
+        <v>4011</v>
+      </c>
+      <c r="R7" s="35">
         <v>3891</v>
       </c>
-      <c r="S7" s="44">
+      <c r="S7" s="35">
         <v>3814</v>
       </c>
-      <c r="T7" s="44">
+      <c r="T7" s="35">
         <v>3522</v>
       </c>
-      <c r="U7" s="44">
+      <c r="U7" s="35">
         <v>3358</v>
       </c>
     </row>
@@ -2064,16 +2099,22 @@
       <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R8" s="44">
+      <c r="P8" s="35">
+        <v>6080</v>
+      </c>
+      <c r="Q8" s="35">
+        <v>5644</v>
+      </c>
+      <c r="R8" s="35">
         <v>5410</v>
       </c>
-      <c r="S8" s="44">
+      <c r="S8" s="35">
         <v>5810</v>
       </c>
-      <c r="T8" s="44">
+      <c r="T8" s="35">
         <v>5350</v>
       </c>
-      <c r="U8" s="44">
+      <c r="U8" s="35">
         <v>5713</v>
       </c>
     </row>
@@ -2081,16 +2122,22 @@
       <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R9" s="44">
+      <c r="P9" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="35">
+        <v>0</v>
+      </c>
+      <c r="R9" s="35">
         <v>575</v>
       </c>
-      <c r="S9" s="44">
+      <c r="S9" s="35">
         <v>660</v>
       </c>
-      <c r="T9" s="44">
+      <c r="T9" s="35">
         <v>664</v>
       </c>
-      <c r="U9" s="44">
+      <c r="U9" s="35">
         <v>561</v>
       </c>
     </row>
@@ -2098,16 +2145,22 @@
       <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="44">
+      <c r="P10" s="35">
+        <v>47</v>
+      </c>
+      <c r="Q10" s="35">
+        <v>-59</v>
+      </c>
+      <c r="R10" s="35">
         <v>-908</v>
       </c>
-      <c r="S10" s="44">
+      <c r="S10" s="35">
         <v>-2505</v>
       </c>
-      <c r="T10" s="44">
+      <c r="T10" s="35">
         <v>342</v>
       </c>
-      <c r="U10" s="44">
+      <c r="U10" s="35">
         <v>211</v>
       </c>
     </row>
@@ -2115,16 +2168,22 @@
       <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="44">
+      <c r="P11" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="35">
+        <v>0</v>
+      </c>
+      <c r="R11" s="35">
         <v>3525</v>
       </c>
-      <c r="S11" s="44">
+      <c r="S11" s="35">
         <v>1685</v>
       </c>
-      <c r="T11" s="44">
+      <c r="T11" s="35">
         <v>0</v>
       </c>
-      <c r="U11" s="44">
+      <c r="U11" s="35">
         <v>0</v>
       </c>
     </row>
@@ -2132,16 +2191,22 @@
       <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R12" s="44">
+      <c r="P12" s="35">
+        <v>1052</v>
+      </c>
+      <c r="Q12" s="35">
+        <v>213</v>
+      </c>
+      <c r="R12" s="35">
         <v>-148</v>
       </c>
-      <c r="S12" s="44">
+      <c r="S12" s="35">
         <v>4281</v>
       </c>
-      <c r="T12" s="44">
+      <c r="T12" s="35">
         <v>568</v>
       </c>
-      <c r="U12" s="44">
+      <c r="U12" s="35">
         <v>79</v>
       </c>
     </row>
@@ -2149,24 +2214,32 @@
       <c r="B13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="R13" s="43">
+      <c r="D13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="P13" s="34">
+        <f t="shared" ref="P13:Q13" si="1">P6-P7-P8-P9+P10-P11+P12</f>
+        <v>3725</v>
+      </c>
+      <c r="Q13" s="34">
+        <f t="shared" si="1"/>
+        <v>4299</v>
+      </c>
+      <c r="R13" s="34">
         <f>R6-R7-R8-R9+R10-R11+R12</f>
         <v>-951</v>
       </c>
-      <c r="S13" s="43">
+      <c r="S13" s="34">
         <f>S6-S7-S8-S9+S10-S11+S12</f>
         <v>4099</v>
       </c>
-      <c r="T13" s="43">
+      <c r="T13" s="34">
         <f>T6-T7-T8-T9+T10-T11+T12</f>
         <v>5097</v>
       </c>
-      <c r="U13" s="43">
+      <c r="U13" s="34">
         <f>U6-U7-U8-U9+U10-U11+U12</f>
         <v>5664</v>
       </c>
@@ -2175,16 +2248,22 @@
       <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="R14" s="44">
+      <c r="P14" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="35">
+        <v>32</v>
+      </c>
+      <c r="R14" s="35">
         <v>7</v>
       </c>
-      <c r="S14" s="44">
+      <c r="S14" s="35">
         <v>3</v>
       </c>
-      <c r="T14" s="44">
+      <c r="T14" s="35">
         <v>0</v>
       </c>
-      <c r="U14" s="44">
+      <c r="U14" s="35">
         <v>0</v>
       </c>
     </row>
@@ -2192,16 +2271,22 @@
       <c r="B15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R15" s="44">
+      <c r="P15" s="35">
+        <v>474</v>
+      </c>
+      <c r="Q15" s="35">
+        <v>685</v>
+      </c>
+      <c r="R15" s="35">
         <v>433</v>
       </c>
-      <c r="S15" s="44">
+      <c r="S15" s="35">
         <v>248</v>
       </c>
-      <c r="T15" s="44">
+      <c r="T15" s="35">
         <v>330</v>
       </c>
-      <c r="U15" s="44">
+      <c r="U15" s="35">
         <v>254</v>
       </c>
     </row>
@@ -2209,16 +2294,22 @@
       <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R16" s="44">
+      <c r="P16" s="35">
+        <v>1406</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>1074</v>
+      </c>
+      <c r="R16" s="35">
         <v>2088</v>
       </c>
-      <c r="S16" s="44">
+      <c r="S16" s="35">
         <v>3549</v>
       </c>
-      <c r="T16" s="44">
+      <c r="T16" s="35">
         <v>1027</v>
       </c>
-      <c r="U16" s="44">
+      <c r="U16" s="35">
         <v>1964</v>
       </c>
     </row>
@@ -2226,19 +2317,27 @@
       <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="R17" s="44">
+      <c r="P17" s="35">
+        <f t="shared" ref="P17:Q17" si="2">P13-P14+P15-P16</f>
+        <v>2792</v>
+      </c>
+      <c r="Q17" s="35">
+        <f t="shared" si="2"/>
+        <v>3878</v>
+      </c>
+      <c r="R17" s="35">
         <f>R13-R14+R15-R16</f>
         <v>-2613</v>
       </c>
-      <c r="S17" s="44">
+      <c r="S17" s="35">
         <f>S13-S14+S15-S16</f>
         <v>795</v>
       </c>
-      <c r="T17" s="44">
+      <c r="T17" s="35">
         <f>T13-T14+T15-T16</f>
         <v>4400</v>
       </c>
-      <c r="U17" s="44">
+      <c r="U17" s="35">
         <f>U13-U14+U15-U16</f>
         <v>3954</v>
       </c>
@@ -2247,16 +2346,22 @@
       <c r="B18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R18" s="44">
+      <c r="P18" s="35">
+        <v>4764</v>
+      </c>
+      <c r="Q18" s="35">
+        <v>-879</v>
+      </c>
+      <c r="R18" s="35">
         <v>1496</v>
       </c>
-      <c r="S18" s="44">
+      <c r="S18" s="35">
         <v>1250</v>
       </c>
-      <c r="T18" s="44">
+      <c r="T18" s="35">
         <v>3864</v>
       </c>
-      <c r="U18" s="44">
+      <c r="U18" s="35">
         <v>1330</v>
       </c>
     </row>
@@ -2264,24 +2369,32 @@
       <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="R19" s="43">
+      <c r="D19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="P19" s="34">
+        <f t="shared" ref="P19:Q19" si="3">P17-P18</f>
+        <v>-1972</v>
+      </c>
+      <c r="Q19" s="34">
+        <f t="shared" si="3"/>
+        <v>4757</v>
+      </c>
+      <c r="R19" s="34">
         <f>R17-R18</f>
         <v>-4109</v>
       </c>
-      <c r="S19" s="43">
+      <c r="S19" s="34">
         <f>S17-S18</f>
         <v>-455</v>
       </c>
-      <c r="T19" s="43">
+      <c r="T19" s="34">
         <f>T17-T18</f>
         <v>536</v>
       </c>
-      <c r="U19" s="43">
+      <c r="U19" s="34">
         <f>U17-U18</f>
         <v>2624</v>
       </c>
@@ -2290,16 +2403,24 @@
       <c r="B20" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="P20" s="1">
+        <f t="shared" ref="P20:R20" si="4">P19/P21</f>
+        <v>-7.0501590933466807E-2</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="4"/>
+        <v>0.17129996398991718</v>
+      </c>
       <c r="R20" s="1">
-        <f t="shared" ref="R20" si="0">R19/R21</f>
+        <f t="shared" si="4"/>
         <v>-0.14883906255659796</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" ref="S20" si="1">S19/S21</f>
+        <f t="shared" ref="S20" si="5">S19/S21</f>
         <v>-1.5454113171659534E-2</v>
       </c>
       <c r="T20" s="1">
-        <f t="shared" ref="T20" si="2">T19/T21</f>
+        <f t="shared" ref="T20" si="6">T19/T21</f>
         <v>1.8113003514463367E-2</v>
       </c>
       <c r="U20" s="1">
@@ -2311,16 +2432,22 @@
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R21" s="44">
+      <c r="P21" s="35">
+        <v>27971</v>
+      </c>
+      <c r="Q21" s="35">
+        <v>27770</v>
+      </c>
+      <c r="R21" s="35">
         <v>27607</v>
       </c>
-      <c r="S21" s="44">
+      <c r="S21" s="35">
         <v>29442</v>
       </c>
-      <c r="T21" s="44">
+      <c r="T21" s="35">
         <v>29592</v>
       </c>
-      <c r="U21" s="44">
+      <c r="U21" s="35">
         <v>29012</v>
       </c>
     </row>
@@ -2328,20 +2455,28 @@
       <c r="B23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="S23" s="46">
-        <f t="shared" ref="S23:U23" si="3">S4/R4-1</f>
+      <c r="D23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="Q23" s="37">
+        <f t="shared" ref="Q23" si="7">Q4/P4-1</f>
+        <v>-2.2254414142050316E-2</v>
+      </c>
+      <c r="R23" s="37">
+        <f t="shared" ref="R23" si="8">R4/Q4-1</f>
+        <v>-6.2377874643018139E-2</v>
+      </c>
+      <c r="S23" s="37">
+        <f t="shared" ref="S23:T23" si="9">S4/R4-1</f>
         <v>2.9954655796271767E-2</v>
       </c>
-      <c r="T23" s="46">
-        <f t="shared" si="3"/>
+      <c r="T23" s="37">
+        <f t="shared" si="9"/>
         <v>-2.5903855560990841E-2</v>
       </c>
-      <c r="U23" s="46">
+      <c r="U23" s="37">
         <f>U4/T4-1</f>
         <v>4.0425483348170532E-2</v>
       </c>
@@ -2355,19 +2490,27 @@
       <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R26" s="47">
-        <f t="shared" ref="R26:T26" si="4">R6/R4</f>
+      <c r="P26" s="38">
+        <f t="shared" ref="P26:Q26" si="10">P6/P4</f>
+        <v>0.27408620436270498</v>
+      </c>
+      <c r="Q26" s="38">
+        <f t="shared" ref="Q26:R26" si="11">Q6/Q4</f>
+        <v>0.29632174529213456</v>
+      </c>
+      <c r="R26" s="38">
+        <f t="shared" ref="R26:S26" si="12">R6/R4</f>
         <v>0.30930243209819996</v>
       </c>
-      <c r="S26" s="47">
-        <f t="shared" si="4"/>
+      <c r="S26" s="38">
+        <f t="shared" si="12"/>
         <v>0.31778360830702185</v>
       </c>
-      <c r="T26" s="47">
-        <f t="shared" ref="T26:U26" si="5">T6/T4</f>
+      <c r="T26" s="38">
+        <f t="shared" ref="T26" si="13">T6/T4</f>
         <v>0.31324613663859024</v>
       </c>
-      <c r="U26" s="47">
+      <c r="U26" s="38">
         <f>U6/U4</f>
         <v>0.32922334357174199</v>
       </c>
@@ -2376,19 +2519,27 @@
       <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="R27" s="47">
-        <f t="shared" ref="R27:T27" si="6">R13/R4</f>
+      <c r="P27" s="38">
+        <f t="shared" ref="P27:Q27" si="14">P13/P4</f>
+        <v>7.8205370452016545E-2</v>
+      </c>
+      <c r="Q27" s="38">
+        <f t="shared" ref="Q27:R27" si="15">Q13/Q4</f>
+        <v>9.2310665435571496E-2</v>
+      </c>
+      <c r="R27" s="38">
+        <f t="shared" ref="R27:S27" si="16">R13/R4</f>
         <v>-2.177895845738103E-2</v>
       </c>
-      <c r="S27" s="47">
-        <f t="shared" si="6"/>
+      <c r="S27" s="38">
+        <f t="shared" si="16"/>
         <v>9.1141548450215687E-2</v>
       </c>
-      <c r="T27" s="47">
-        <f t="shared" ref="T27:U27" si="7">T13/T4</f>
+      <c r="T27" s="38">
+        <f t="shared" ref="T27" si="17">T13/T4</f>
         <v>0.11634595631034719</v>
       </c>
-      <c r="U27" s="47">
+      <c r="U27" s="38">
         <f>U13/U4</f>
         <v>0.12426502852128127</v>
       </c>
@@ -2397,19 +2548,27 @@
       <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R28" s="47">
-        <f t="shared" ref="R28:T28" si="8">R19/R4</f>
+      <c r="P28" s="38">
+        <f t="shared" ref="P28:Q28" si="18">P19/P4</f>
+        <v>-4.1401608196342719E-2</v>
+      </c>
+      <c r="Q28" s="38">
+        <f t="shared" ref="Q28:R28" si="19">Q19/Q4</f>
+        <v>0.10214511176483219</v>
+      </c>
+      <c r="R28" s="38">
+        <f t="shared" ref="R28:S28" si="20">R19/R4</f>
         <v>-9.4100673292722023E-2</v>
       </c>
-      <c r="S28" s="47">
-        <f t="shared" si="8"/>
+      <c r="S28" s="38">
+        <f t="shared" si="20"/>
         <v>-1.0116956463734603E-2</v>
       </c>
-      <c r="T28" s="47">
-        <f t="shared" ref="T28:U28" si="9">T19/T4</f>
+      <c r="T28" s="38">
+        <f t="shared" ref="T28" si="21">T19/T4</f>
         <v>1.2234928895888973E-2</v>
       </c>
-      <c r="U28" s="47">
+      <c r="U28" s="38">
         <f>U19/U4</f>
         <v>5.7569109258446688E-2</v>
       </c>
@@ -2418,25 +2577,33 @@
       <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R29" s="47">
-        <f t="shared" ref="R29:T29" si="10">R19/R4</f>
+      <c r="P29" s="38">
+        <f t="shared" ref="P29:Q29" si="22">P19/P4</f>
+        <v>-4.1401608196342719E-2</v>
+      </c>
+      <c r="Q29" s="38">
+        <f t="shared" ref="Q29:R29" si="23">Q19/Q4</f>
+        <v>0.10214511176483219</v>
+      </c>
+      <c r="R29" s="38">
+        <f t="shared" ref="R29:S29" si="24">R19/R4</f>
         <v>-9.4100673292722023E-2</v>
       </c>
-      <c r="S29" s="47">
-        <f t="shared" si="10"/>
+      <c r="S29" s="38">
+        <f t="shared" si="24"/>
         <v>-1.0116956463734603E-2</v>
       </c>
-      <c r="T29" s="47">
-        <f t="shared" ref="T29:U29" si="11">T19/T4</f>
+      <c r="T29" s="38">
+        <f t="shared" ref="T29" si="25">T19/T4</f>
         <v>1.2234928895888973E-2</v>
       </c>
-      <c r="U29" s="47">
+      <c r="U29" s="38">
         <f>U19/U4</f>
         <v>5.7569109258446688E-2</v>
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="39" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2444,19 +2611,27 @@
       <c r="B34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="R34" s="44">
+      <c r="P34" s="35">
+        <f>26808+19412</f>
+        <v>46220</v>
+      </c>
+      <c r="Q34" s="35">
+        <f>26734+16523</f>
+        <v>43257</v>
+      </c>
+      <c r="R34" s="35">
         <f>23353+17652</f>
         <v>41005</v>
       </c>
-      <c r="S34" s="44">
+      <c r="S34" s="35">
         <f>31271+22252</f>
         <v>53523</v>
       </c>
-      <c r="T34" s="44">
+      <c r="T34" s="35">
         <f>31731+21818</f>
         <v>53549</v>
       </c>
-      <c r="U34" s="44">
+      <c r="U34" s="35">
         <f>31884+21360</f>
         <v>53244</v>
       </c>
@@ -2465,16 +2640,22 @@
       <c r="B35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R35" s="44">
+      <c r="P35" s="35">
+        <v>30204</v>
+      </c>
+      <c r="Q35" s="35">
+        <v>28325</v>
+      </c>
+      <c r="R35" s="35">
         <v>27432</v>
       </c>
-      <c r="S35" s="44">
+      <c r="S35" s="35">
         <v>39197</v>
       </c>
-      <c r="T35" s="44">
+      <c r="T35" s="35">
         <v>41243</v>
       </c>
-      <c r="U35" s="44">
+      <c r="U35" s="35">
         <v>40804</v>
       </c>
     </row>
@@ -2482,16 +2663,22 @@
       <c r="B36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="R36" s="44">
+      <c r="P36" s="35">
+        <v>3138</v>
+      </c>
+      <c r="Q36" s="35">
+        <v>2538</v>
+      </c>
+      <c r="R36" s="35">
         <v>3952</v>
       </c>
-      <c r="S36" s="44">
+      <c r="S36" s="35">
         <v>5831</v>
       </c>
-      <c r="T36" s="44">
+      <c r="T36" s="35">
         <v>4670</v>
       </c>
-      <c r="U36" s="44">
+      <c r="U36" s="35">
         <v>4268</v>
       </c>
     </row>
@@ -2499,16 +2686,22 @@
       <c r="B37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R37" s="44">
+      <c r="P37" s="35">
+        <v>3459</v>
+      </c>
+      <c r="Q37" s="35">
+        <v>3204</v>
+      </c>
+      <c r="R37" s="35">
         <v>870</v>
       </c>
-      <c r="S37" s="44">
+      <c r="S37" s="35">
         <v>792</v>
       </c>
-      <c r="T37" s="44">
+      <c r="T37" s="35">
         <v>925</v>
       </c>
-      <c r="U37" s="44">
+      <c r="U37" s="35">
         <v>1073</v>
       </c>
     </row>
@@ -2516,16 +2709,22 @@
       <c r="B38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="R38" s="44">
+      <c r="P38" s="35">
+        <v>24300</v>
+      </c>
+      <c r="Q38" s="35">
+        <v>26200</v>
+      </c>
+      <c r="R38" s="35">
         <v>24753</v>
       </c>
-      <c r="S38" s="44">
+      <c r="S38" s="35">
         <v>23606</v>
       </c>
-      <c r="T38" s="44">
+      <c r="T38" s="35">
         <v>21569</v>
       </c>
-      <c r="U38" s="44">
+      <c r="U38" s="35">
         <v>19089</v>
       </c>
     </row>
@@ -2533,16 +2732,22 @@
       <c r="B39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R39" s="44">
+      <c r="P39" s="35">
+        <v>57</v>
+      </c>
+      <c r="Q39" s="35">
+        <v>110</v>
+      </c>
+      <c r="R39" s="35">
         <v>94</v>
       </c>
-      <c r="S39" s="44">
+      <c r="S39" s="35">
         <v>590</v>
       </c>
-      <c r="T39" s="44">
+      <c r="T39" s="35">
         <v>60</v>
       </c>
-      <c r="U39" s="44">
+      <c r="U39" s="35">
         <v>555</v>
       </c>
     </row>
@@ -2550,16 +2755,22 @@
       <c r="B40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="R40" s="44">
+      <c r="P40" s="35">
+        <v>4569</v>
+      </c>
+      <c r="Q40" s="35">
+        <v>4026</v>
+      </c>
+      <c r="R40" s="35">
         <v>5170</v>
       </c>
-      <c r="S40" s="44">
+      <c r="S40" s="35">
         <v>10378</v>
       </c>
-      <c r="T40" s="44">
+      <c r="T40" s="35">
         <v>4777</v>
       </c>
-      <c r="U40" s="44">
+      <c r="U40" s="35">
         <v>6383</v>
       </c>
     </row>
@@ -2567,19 +2778,27 @@
       <c r="B41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R41" s="44">
+      <c r="P41" s="35">
+        <f>SUM(P34:P40)</f>
+        <v>111947</v>
+      </c>
+      <c r="Q41" s="35">
+        <f>SUM(Q34:Q40)</f>
+        <v>107660</v>
+      </c>
+      <c r="R41" s="35">
         <f>SUM(R34:R40)</f>
         <v>103276</v>
       </c>
-      <c r="S41" s="44">
+      <c r="S41" s="35">
         <f>SUM(S34:S40)</f>
         <v>133917</v>
       </c>
-      <c r="T41" s="44">
+      <c r="T41" s="35">
         <f>SUM(T34:T40)</f>
         <v>126793</v>
       </c>
-      <c r="U41" s="44">
+      <c r="U41" s="35">
         <f>SUM(U34:U40)</f>
         <v>125416</v>
       </c>
@@ -2588,21 +2807,27 @@
       <c r="B42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="L42" s="41"/>
-      <c r="R42" s="43">
+      <c r="D42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="P42" s="34">
+        <v>576</v>
+      </c>
+      <c r="Q42" s="34">
+        <v>581</v>
+      </c>
+      <c r="R42" s="34">
         <v>714</v>
       </c>
-      <c r="S42" s="43">
+      <c r="S42" s="34">
         <v>585</v>
       </c>
-      <c r="T42" s="43">
+      <c r="T42" s="34">
         <v>676</v>
       </c>
-      <c r="U42" s="43">
+      <c r="U42" s="34">
         <v>836</v>
       </c>
     </row>
@@ -2610,16 +2835,22 @@
       <c r="B43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R43" s="44">
+      <c r="P43" s="35">
+        <v>150</v>
+      </c>
+      <c r="Q43" s="35">
+        <v>106</v>
+      </c>
+      <c r="R43" s="35">
         <v>264</v>
       </c>
-      <c r="S43" s="44">
+      <c r="S43" s="35">
         <v>275</v>
       </c>
-      <c r="T43" s="44">
+      <c r="T43" s="35">
         <v>434</v>
       </c>
-      <c r="U43" s="44">
+      <c r="U43" s="35">
         <v>296</v>
       </c>
     </row>
@@ -2627,16 +2858,22 @@
       <c r="B44" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="R44" s="44">
+      <c r="P44" s="35">
+        <v>9861</v>
+      </c>
+      <c r="Q44" s="35">
+        <v>9975</v>
+      </c>
+      <c r="R44" s="35">
         <v>12190</v>
       </c>
-      <c r="S44" s="44">
+      <c r="S44" s="35">
         <v>11411</v>
       </c>
-      <c r="T44" s="44">
+      <c r="T44" s="35">
         <v>10923</v>
       </c>
-      <c r="U44" s="44">
+      <c r="U44" s="35">
         <v>11019</v>
       </c>
     </row>
@@ -2644,16 +2881,22 @@
       <c r="B45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R45" s="44">
+      <c r="P45" s="35">
+        <v>6120</v>
+      </c>
+      <c r="Q45" s="35">
+        <v>8795</v>
+      </c>
+      <c r="R45" s="35">
         <v>13012</v>
       </c>
-      <c r="S45" s="44">
+      <c r="S45" s="35">
         <v>7089</v>
       </c>
-      <c r="T45" s="44">
+      <c r="T45" s="35">
         <v>9159</v>
       </c>
-      <c r="U45" s="44">
+      <c r="U45" s="35">
         <v>7931</v>
       </c>
     </row>
@@ -2661,21 +2904,27 @@
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="R46" s="43">
+      <c r="D46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="P46" s="34">
+        <v>8835</v>
+      </c>
+      <c r="Q46" s="34">
+        <v>4674</v>
+      </c>
+      <c r="R46" s="34">
         <v>13637</v>
       </c>
-      <c r="S46" s="43">
+      <c r="S46" s="34">
         <v>13284</v>
       </c>
-      <c r="T46" s="43">
+      <c r="T46" s="34">
         <v>5821</v>
       </c>
-      <c r="U46" s="43">
+      <c r="U46" s="34">
         <v>7496</v>
       </c>
     </row>
@@ -2683,16 +2932,22 @@
       <c r="B47" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R47" s="44">
+      <c r="P47" s="35">
+        <v>17195</v>
+      </c>
+      <c r="Q47" s="35">
+        <v>13820</v>
+      </c>
+      <c r="R47" s="35">
         <v>-231</v>
       </c>
-      <c r="S47" s="44">
+      <c r="S47" s="35">
         <v>1607</v>
       </c>
-      <c r="T47" s="44">
+      <c r="T47" s="35">
         <v>1257</v>
       </c>
-      <c r="U47" s="44">
+      <c r="U47" s="35">
         <v>959</v>
       </c>
     </row>
@@ -2700,19 +2955,27 @@
       <c r="B48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="R48" s="44">
+      <c r="P48" s="35">
+        <f>P41+SUM(P42:P47)</f>
+        <v>154684</v>
+      </c>
+      <c r="Q48" s="35">
+        <f>Q41+SUM(Q42:Q47)</f>
+        <v>145611</v>
+      </c>
+      <c r="R48" s="35">
         <f>R41+SUM(R42:R47)</f>
         <v>142862</v>
       </c>
-      <c r="S48" s="44">
+      <c r="S48" s="35">
         <f>S41+SUM(S42:S47)</f>
         <v>168168</v>
       </c>
-      <c r="T48" s="44">
+      <c r="T48" s="35">
         <f>T41+SUM(T42:T47)</f>
         <v>155063</v>
       </c>
-      <c r="U48" s="44">
+      <c r="U48" s="35">
         <f>U41+SUM(U42:U47)</f>
         <v>153953</v>
       </c>
@@ -2721,21 +2984,27 @@
       <c r="B50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="J50" s="41"/>
-      <c r="L50" s="41"/>
-      <c r="R50" s="43">
+      <c r="D50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="P50" s="34">
+        <v>34523</v>
+      </c>
+      <c r="Q50" s="34">
+        <v>32908</v>
+      </c>
+      <c r="R50" s="34">
         <v>48685</v>
       </c>
-      <c r="S50" s="43">
+      <c r="S50" s="34">
         <v>62892</v>
       </c>
-      <c r="T50" s="43">
+      <c r="T50" s="34">
         <v>59272</v>
       </c>
-      <c r="U50" s="43">
+      <c r="U50" s="34">
         <v>58131</v>
       </c>
     </row>
@@ -2743,16 +3012,22 @@
       <c r="B51" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="R51" s="44">
+      <c r="P51" s="35">
+        <v>535</v>
+      </c>
+      <c r="Q51" s="35">
+        <v>644</v>
+      </c>
+      <c r="R51" s="35">
         <v>478</v>
       </c>
-      <c r="S51" s="44">
+      <c r="S51" s="35">
         <v>2043</v>
       </c>
-      <c r="T51" s="44">
+      <c r="T51" s="35">
         <v>2095</v>
       </c>
-      <c r="U51" s="44">
+      <c r="U51" s="35">
         <v>520</v>
       </c>
     </row>
@@ -2760,16 +3035,22 @@
       <c r="B52" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R52" s="44">
+      <c r="P52" s="35">
+        <v>651</v>
+      </c>
+      <c r="Q52" s="35">
+        <v>520</v>
+      </c>
+      <c r="R52" s="35">
         <v>551</v>
       </c>
-      <c r="S52" s="44">
+      <c r="S52" s="35">
         <v>438</v>
       </c>
-      <c r="T52" s="44">
+      <c r="T52" s="35">
         <v>513</v>
       </c>
-      <c r="U52" s="44">
+      <c r="U52" s="35">
         <v>281</v>
       </c>
     </row>
@@ -2777,16 +3058,22 @@
       <c r="B53" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R53" s="44">
+      <c r="P53" s="35">
+        <v>1130</v>
+      </c>
+      <c r="Q53" s="35">
+        <v>1065</v>
+      </c>
+      <c r="R53" s="35">
         <v>1242</v>
       </c>
-      <c r="S53" s="44">
+      <c r="S53" s="35">
         <v>1474</v>
       </c>
-      <c r="T53" s="44">
+      <c r="T53" s="35">
         <v>1747</v>
       </c>
-      <c r="U53" s="44">
+      <c r="U53" s="35">
         <v>1881</v>
       </c>
     </row>
@@ -2794,16 +3081,22 @@
       <c r="B54" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R54" s="44">
+      <c r="P54" s="35">
+        <v>1737</v>
+      </c>
+      <c r="Q54" s="35">
+        <v>2843</v>
+      </c>
+      <c r="R54" s="35">
         <v>2938</v>
       </c>
-      <c r="S54" s="44">
+      <c r="S54" s="35">
         <v>5189</v>
       </c>
-      <c r="T54" s="44">
+      <c r="T54" s="35">
         <v>4909</v>
       </c>
-      <c r="U54" s="44">
+      <c r="U54" s="35">
         <v>2516</v>
       </c>
     </row>
@@ -2811,19 +3104,27 @@
       <c r="B55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R55" s="44">
+      <c r="P55" s="35">
+        <f>SUM(P50:P54)</f>
+        <v>38576</v>
+      </c>
+      <c r="Q55" s="35">
+        <f>SUM(Q50:Q54)</f>
+        <v>37980</v>
+      </c>
+      <c r="R55" s="35">
         <f>SUM(R50:R54)</f>
         <v>53894</v>
       </c>
-      <c r="S55" s="44">
+      <c r="S55" s="35">
         <f>SUM(S50:S54)</f>
         <v>72036</v>
       </c>
-      <c r="T55" s="44">
+      <c r="T55" s="35">
         <f>SUM(T50:T54)</f>
         <v>68536</v>
       </c>
-      <c r="U55" s="44">
+      <c r="U55" s="35">
         <f>SUM(U50:U54)</f>
         <v>63329</v>
       </c>
@@ -2832,21 +3133,27 @@
       <c r="B56" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="L56" s="41"/>
-      <c r="R56" s="43">
+      <c r="D56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="L56" s="32"/>
+      <c r="P56" s="34">
+        <v>12051</v>
+      </c>
+      <c r="Q56" s="34">
+        <v>10351</v>
+      </c>
+      <c r="R56" s="34">
         <v>4270</v>
       </c>
-      <c r="S56" s="43">
+      <c r="S56" s="34">
         <v>11826</v>
       </c>
-      <c r="T56" s="43">
+      <c r="T56" s="34">
         <v>8488</v>
       </c>
-      <c r="U56" s="43">
+      <c r="U56" s="34">
         <v>11961</v>
       </c>
     </row>
@@ -2854,21 +3161,27 @@
       <c r="B57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="J57" s="41"/>
-      <c r="L57" s="41"/>
-      <c r="R57" s="43">
+      <c r="D57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="L57" s="32"/>
+      <c r="P57" s="34">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="34">
+        <v>0</v>
+      </c>
+      <c r="R57" s="34">
         <v>1844</v>
       </c>
-      <c r="S57" s="43">
+      <c r="S57" s="34">
         <v>1850</v>
       </c>
-      <c r="T57" s="43">
+      <c r="T57" s="34">
         <v>492</v>
       </c>
-      <c r="U57" s="43">
+      <c r="U57" s="34">
         <v>494</v>
       </c>
     </row>
@@ -2876,16 +3189,22 @@
       <c r="B58" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R58" s="44">
+      <c r="P58" s="34">
+        <v>661</v>
+      </c>
+      <c r="Q58" s="35">
+        <v>541</v>
+      </c>
+      <c r="R58" s="35">
         <v>596</v>
       </c>
-      <c r="S58" s="44">
+      <c r="S58" s="35">
         <v>671</v>
       </c>
-      <c r="T58" s="44">
+      <c r="T58" s="35">
         <v>769</v>
       </c>
-      <c r="U58" s="44">
+      <c r="U58" s="35">
         <v>864</v>
       </c>
     </row>
@@ -2893,16 +3212,22 @@
       <c r="B59" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="R59" s="44">
+      <c r="P59" s="35">
+        <v>1049</v>
+      </c>
+      <c r="Q59" s="35">
+        <v>891</v>
+      </c>
+      <c r="R59" s="35">
         <v>1160</v>
       </c>
-      <c r="S59" s="44">
+      <c r="S59" s="35">
         <v>1024</v>
       </c>
-      <c r="T59" s="44">
+      <c r="T59" s="35">
         <v>892</v>
       </c>
-      <c r="U59" s="44">
+      <c r="U59" s="35">
         <v>667</v>
       </c>
     </row>
@@ -2910,16 +3235,22 @@
       <c r="B60" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="R60" s="44">
+      <c r="P60" s="35">
+        <v>16834</v>
+      </c>
+      <c r="Q60" s="35">
+        <v>16242</v>
+      </c>
+      <c r="R60" s="35">
         <v>17653</v>
       </c>
-      <c r="S60" s="44">
+      <c r="S60" s="35">
         <v>17085</v>
       </c>
-      <c r="T60" s="44">
+      <c r="T60" s="35">
         <v>18070</v>
       </c>
-      <c r="U60" s="44">
+      <c r="U60" s="35">
         <v>19661</v>
       </c>
     </row>
@@ -2927,19 +3258,27 @@
       <c r="B61" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R61" s="44">
+      <c r="P61" s="35">
+        <f>P55+SUM(P56:P60)</f>
+        <v>69171</v>
+      </c>
+      <c r="Q61" s="35">
+        <f>Q55+SUM(Q56:Q60)</f>
+        <v>66005</v>
+      </c>
+      <c r="R61" s="35">
         <f>R55+SUM(R56:R60)</f>
         <v>79417</v>
       </c>
-      <c r="S61" s="44">
+      <c r="S61" s="35">
         <f>S55+SUM(S56:S60)</f>
         <v>104492</v>
       </c>
-      <c r="T61" s="44">
+      <c r="T61" s="35">
         <f>T55+SUM(T56:T60)</f>
         <v>97247</v>
       </c>
-      <c r="U61" s="44">
+      <c r="U61" s="35">
         <f>U55+SUM(U56:U60)</f>
         <v>96976</v>
       </c>
@@ -2948,16 +3287,22 @@
       <c r="B63" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R63" s="44">
+      <c r="P63" s="35">
+        <v>73719</v>
+      </c>
+      <c r="Q63" s="35">
+        <v>68607</v>
+      </c>
+      <c r="R63" s="35">
         <v>63445</v>
       </c>
-      <c r="S63" s="44">
+      <c r="S63" s="35">
         <v>62625</v>
       </c>
-      <c r="T63" s="44">
+      <c r="T63" s="35">
         <v>57816</v>
       </c>
-      <c r="U63" s="44">
+      <c r="U63" s="35">
         <v>56977</v>
       </c>
     </row>
@@ -2965,19 +3310,27 @@
       <c r="B64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R64" s="44">
+      <c r="P64" s="35">
+        <f t="shared" ref="P64:Q64" si="26">P63+P61</f>
+        <v>142890</v>
+      </c>
+      <c r="Q64" s="35">
+        <f t="shared" si="26"/>
+        <v>134612</v>
+      </c>
+      <c r="R64" s="35">
         <f>R63+R61</f>
         <v>142862</v>
       </c>
-      <c r="S64" s="44">
+      <c r="S64" s="35">
         <f>S63+S61</f>
         <v>167117</v>
       </c>
-      <c r="T64" s="44">
+      <c r="T64" s="35">
         <f>T63+T61</f>
         <v>155063</v>
       </c>
-      <c r="U64" s="44">
+      <c r="U64" s="35">
         <f>U63+U61</f>
         <v>153953</v>
       </c>
@@ -2986,19 +3339,27 @@
       <c r="B66" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="R66" s="44">
-        <f t="shared" ref="R66:S66" si="12">R48-R61</f>
+      <c r="P66" s="35">
+        <f t="shared" ref="P66:R66" si="27">P48-P61</f>
+        <v>85513</v>
+      </c>
+      <c r="Q66" s="35">
+        <f t="shared" si="27"/>
+        <v>79606</v>
+      </c>
+      <c r="R66" s="35">
+        <f t="shared" si="27"/>
         <v>63445</v>
       </c>
-      <c r="S66" s="44">
-        <f t="shared" ref="S66:T66" si="13">S48-S61</f>
+      <c r="S66" s="35">
+        <f t="shared" ref="S66" si="28">S48-S61</f>
         <v>63676</v>
       </c>
-      <c r="T66" s="44">
+      <c r="T66" s="35">
         <f>T48-T61</f>
         <v>57816</v>
       </c>
-      <c r="U66" s="44">
+      <c r="U66" s="35">
         <f>U48-U61</f>
         <v>56977</v>
       </c>
@@ -3007,12 +3368,20 @@
       <c r="B67" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="P67" s="1">
+        <f t="shared" ref="P67:R67" si="29">P66/P21</f>
+        <v>3.0572021021772549</v>
+      </c>
+      <c r="Q67" s="1">
+        <f t="shared" si="29"/>
+        <v>2.8666186532229023</v>
+      </c>
       <c r="R67" s="1">
-        <f t="shared" ref="R67" si="14">R66/R21</f>
+        <f t="shared" si="29"/>
         <v>2.2981490201760422</v>
       </c>
       <c r="S67" s="1">
-        <f t="shared" ref="S67" si="15">S66/S21</f>
+        <f t="shared" ref="S67" si="30">S66/S21</f>
         <v>2.1627606820188845</v>
       </c>
       <c r="T67" s="1">
@@ -3028,15 +3397,23 @@
       <c r="B69" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S69" s="47">
-        <f t="shared" ref="S69:U69" si="16">S42/R42-1</f>
+      <c r="Q69" s="38">
+        <f t="shared" ref="Q69" si="31">Q42/P42-1</f>
+        <v>8.6805555555555802E-3</v>
+      </c>
+      <c r="R69" s="38">
+        <f t="shared" ref="R69" si="32">R42/Q42-1</f>
+        <v>0.22891566265060237</v>
+      </c>
+      <c r="S69" s="38">
+        <f t="shared" ref="S69:T69" si="33">S42/R42-1</f>
         <v>-0.18067226890756305</v>
       </c>
-      <c r="T69" s="47">
-        <f t="shared" si="16"/>
+      <c r="T69" s="38">
+        <f t="shared" si="33"/>
         <v>0.15555555555555545</v>
       </c>
-      <c r="U69" s="47">
+      <c r="U69" s="38">
         <f>U42/T42-1</f>
         <v>0.23668639053254448</v>
       </c>
@@ -3046,54 +3423,70 @@
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="49" t="s">
+    <row r="72" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="H72" s="50"/>
-      <c r="J72" s="50"/>
-      <c r="L72" s="50"/>
-      <c r="R72" s="51">
-        <f t="shared" ref="R72:S72" si="17">R46</f>
+      <c r="D72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="H72" s="41"/>
+      <c r="J72" s="41"/>
+      <c r="L72" s="41"/>
+      <c r="P72" s="42">
+        <f t="shared" ref="P72:R72" si="34">P46</f>
+        <v>8835</v>
+      </c>
+      <c r="Q72" s="42">
+        <f t="shared" si="34"/>
+        <v>4674</v>
+      </c>
+      <c r="R72" s="42">
+        <f t="shared" si="34"/>
         <v>13637</v>
       </c>
-      <c r="S72" s="51">
-        <f t="shared" ref="S72:T72" si="18">S46</f>
+      <c r="S72" s="42">
+        <f t="shared" ref="S72" si="35">S46</f>
         <v>13284</v>
       </c>
-      <c r="T72" s="51">
-        <f t="shared" ref="T72:U72" si="19">T46</f>
+      <c r="T72" s="42">
+        <f t="shared" ref="T72" si="36">T46</f>
         <v>5821</v>
       </c>
-      <c r="U72" s="51">
+      <c r="U72" s="42">
         <f>U46</f>
         <v>7496</v>
       </c>
     </row>
-    <row r="73" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="49" t="s">
+    <row r="73" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="J73" s="50"/>
-      <c r="L73" s="50"/>
-      <c r="R73" s="51">
-        <f t="shared" ref="R73:S73" si="20">R50+R56+R57</f>
+      <c r="D73" s="41"/>
+      <c r="F73" s="41"/>
+      <c r="H73" s="41"/>
+      <c r="J73" s="41"/>
+      <c r="L73" s="41"/>
+      <c r="P73" s="42">
+        <f t="shared" ref="P73:R73" si="37">P50+P56+P57</f>
+        <v>46574</v>
+      </c>
+      <c r="Q73" s="42">
+        <f t="shared" si="37"/>
+        <v>43259</v>
+      </c>
+      <c r="R73" s="42">
+        <f t="shared" si="37"/>
         <v>54799</v>
       </c>
-      <c r="S73" s="51">
-        <f t="shared" ref="S73:T73" si="21">S50+S56+S57</f>
+      <c r="S73" s="42">
+        <f t="shared" ref="S73" si="38">S50+S56+S57</f>
         <v>76568</v>
       </c>
-      <c r="T73" s="51">
-        <f t="shared" ref="T73:U73" si="22">T50+T56+T57</f>
+      <c r="T73" s="42">
+        <f t="shared" ref="T73" si="39">T50+T56+T57</f>
         <v>68252</v>
       </c>
-      <c r="U73" s="51">
+      <c r="U73" s="42">
         <f>U50+U56+U57</f>
         <v>70586</v>
       </c>
@@ -3102,46 +3495,62 @@
       <c r="B74" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R74" s="44">
-        <f t="shared" ref="R74" si="23">R72-R73</f>
+      <c r="P74" s="35">
+        <f t="shared" ref="P74:R74" si="40">P72-P73</f>
+        <v>-37739</v>
+      </c>
+      <c r="Q74" s="35">
+        <f t="shared" si="40"/>
+        <v>-38585</v>
+      </c>
+      <c r="R74" s="35">
+        <f t="shared" si="40"/>
         <v>-41162</v>
       </c>
-      <c r="S74" s="44">
-        <f t="shared" ref="S74" si="24">S72-S73</f>
+      <c r="S74" s="35">
+        <f t="shared" ref="S74" si="41">S72-S73</f>
         <v>-63284</v>
       </c>
-      <c r="T74" s="44">
-        <f t="shared" ref="T74" si="25">T72-T73</f>
+      <c r="T74" s="35">
+        <f t="shared" ref="T74" si="42">T72-T73</f>
         <v>-62431</v>
       </c>
-      <c r="U74" s="44">
+      <c r="U74" s="35">
         <f>U72-U73</f>
         <v>-63090</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
-      <c r="B75" s="53" t="s">
+    <row r="75" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="43"/>
+      <c r="B75" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="D75" s="57"/>
-      <c r="F75" s="57"/>
-      <c r="H75" s="57"/>
-      <c r="J75" s="57"/>
-      <c r="L75" s="57"/>
-      <c r="R75" s="58">
-        <f t="shared" ref="R75" si="26">R74*R81</f>
+      <c r="D75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="H75" s="48"/>
+      <c r="J75" s="48"/>
+      <c r="L75" s="48"/>
+      <c r="P75" s="49">
+        <f t="shared" ref="P75:R75" si="43">P74*P81</f>
+        <v>-32323.453500000003</v>
+      </c>
+      <c r="Q75" s="49">
+        <f t="shared" si="43"/>
+        <v>-33835.186500000003</v>
+      </c>
+      <c r="R75" s="49">
+        <f t="shared" si="43"/>
         <v>-35407.5524</v>
       </c>
-      <c r="S75" s="58">
-        <f t="shared" ref="S75" si="27">S74*S81</f>
+      <c r="S75" s="49">
+        <f t="shared" ref="S75" si="44">S74*S81</f>
         <v>-56411.357599999996</v>
       </c>
-      <c r="T75" s="58">
-        <f t="shared" ref="T75" si="28">T74*T81</f>
+      <c r="T75" s="49">
+        <f t="shared" ref="T75" si="45">T74*T81</f>
         <v>-53241.156799999997</v>
       </c>
-      <c r="U75" s="58">
+      <c r="U75" s="49">
         <f>U74*U81</f>
         <v>-53582.337000000007</v>
       </c>
@@ -3150,6 +3559,12 @@
       <c r="B77" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="P77" s="1">
+        <v>2.081</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>1.9421999999999999</v>
+      </c>
       <c r="R77" s="1">
         <v>1.1020000000000001</v>
       </c>
@@ -3167,19 +3582,27 @@
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R78" s="59">
-        <f t="shared" ref="R78" si="29">R77*R21</f>
+      <c r="P78" s="50">
+        <f t="shared" ref="P78:R78" si="46">P77*P21</f>
+        <v>58207.650999999998</v>
+      </c>
+      <c r="Q78" s="50">
+        <f t="shared" si="46"/>
+        <v>53934.894</v>
+      </c>
+      <c r="R78" s="50">
+        <f t="shared" si="46"/>
         <v>30422.914000000004</v>
       </c>
-      <c r="S78" s="59">
-        <f t="shared" ref="S78" si="30">S77*S21</f>
+      <c r="S78" s="50">
+        <f t="shared" ref="S78" si="47">S77*S21</f>
         <v>33663.982799999998</v>
       </c>
-      <c r="T78" s="59">
-        <f t="shared" ref="T78" si="31">T77*T21</f>
+      <c r="T78" s="50">
+        <f t="shared" ref="T78" si="48">T77*T21</f>
         <v>39025.929599999996</v>
       </c>
-      <c r="U78" s="59">
+      <c r="U78" s="50">
         <f>U77*U21</f>
         <v>36218.580799999996</v>
       </c>
@@ -3188,19 +3611,27 @@
       <c r="B79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R79" s="59">
-        <f t="shared" ref="R79" si="32">R78-R75</f>
+      <c r="P79" s="50">
+        <f t="shared" ref="P79:R79" si="49">P78-P75</f>
+        <v>90531.104500000001</v>
+      </c>
+      <c r="Q79" s="50">
+        <f t="shared" si="49"/>
+        <v>87770.080500000011</v>
+      </c>
+      <c r="R79" s="50">
+        <f t="shared" si="49"/>
         <v>65830.466400000005</v>
       </c>
-      <c r="S79" s="59">
-        <f t="shared" ref="S79" si="33">S78-S75</f>
+      <c r="S79" s="50">
+        <f t="shared" ref="S79" si="50">S78-S75</f>
         <v>90075.340399999986</v>
       </c>
-      <c r="T79" s="59">
-        <f t="shared" ref="T79" si="34">T78-T75</f>
+      <c r="T79" s="50">
+        <f t="shared" ref="T79" si="51">T78-T75</f>
         <v>92267.0864</v>
       </c>
-      <c r="U79" s="59">
+      <c r="U79" s="50">
         <f>U78-U75</f>
         <v>89800.917799999996</v>
       </c>
@@ -3209,6 +3640,12 @@
       <c r="B81" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="P81" s="1">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0.87690000000000001</v>
+      </c>
       <c r="R81" s="1">
         <v>0.86019999999999996</v>
       </c>
@@ -3226,19 +3663,27 @@
       <c r="B83" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R83" s="63">
-        <f t="shared" ref="R83:U83" si="35">R77/R67</f>
+      <c r="P83" s="52">
+        <f t="shared" ref="P83:R83" si="52">P77/P67</f>
+        <v>0.68068774338404692</v>
+      </c>
+      <c r="Q83" s="52">
+        <f t="shared" si="52"/>
+        <v>0.67752297565510133</v>
+      </c>
+      <c r="R83" s="52">
+        <f t="shared" ref="R83:T83" si="53">R77/R67</f>
         <v>0.47951633698479007</v>
       </c>
-      <c r="S83" s="63">
-        <f t="shared" si="35"/>
+      <c r="S83" s="52">
+        <f t="shared" si="53"/>
         <v>0.52867615428104786</v>
       </c>
-      <c r="T83" s="63">
-        <f t="shared" si="35"/>
+      <c r="T83" s="52">
+        <f t="shared" si="53"/>
         <v>0.67500224159402245</v>
       </c>
-      <c r="U83" s="63">
+      <c r="U83" s="52">
         <f>U77/U67</f>
         <v>0.6356701967460554</v>
       </c>
@@ -3247,19 +3692,27 @@
       <c r="B85" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R85" s="63">
-        <f t="shared" ref="R85:U85" si="36">R77/R20</f>
+      <c r="P85" s="52">
+        <f t="shared" ref="P85:R85" si="54">P77/P20</f>
+        <v>-29.517064401622715</v>
+      </c>
+      <c r="Q85" s="52">
+        <f t="shared" si="54"/>
+        <v>11.338005886062644</v>
+      </c>
+      <c r="R85" s="52">
+        <f t="shared" ref="R85:T85" si="55">R77/R20</f>
         <v>-7.4039703090776356</v>
       </c>
-      <c r="S85" s="63">
-        <f t="shared" si="36"/>
+      <c r="S85" s="52">
+        <f t="shared" si="55"/>
         <v>-73.986775384615385</v>
       </c>
-      <c r="T85" s="63">
-        <f t="shared" si="36"/>
+      <c r="T85" s="52">
+        <f t="shared" si="55"/>
         <v>72.80957014925373</v>
       </c>
-      <c r="U85" s="63">
+      <c r="U85" s="52">
         <f>U77/U20</f>
         <v>13.802812804878048</v>
       </c>
@@ -3268,9 +3721,10 @@
   <hyperlinks>
     <hyperlink ref="U1" r:id="rId1" xr:uid="{53B5965E-86A4-4E15-BCC8-BF2778F38F41}"/>
     <hyperlink ref="S1" r:id="rId2" xr:uid="{8A9C1835-76D0-4B4E-98C1-AEE2CB23015C}"/>
+    <hyperlink ref="Q1" r:id="rId3" xr:uid="{43B28802-E1F3-4DFC-9E35-ACFDECE05BD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add revenue segmentation to £VOD
</commit_message>
<xml_diff>
--- a/£VOD.xlsx
+++ b/£VOD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65873D97-D29C-4D88-816B-06531D9366DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE66C550-E015-4BD8-933C-00466F02473C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{5E4D6509-12BB-42E6-9952-4B32877F48D2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="110">
   <si>
     <t>£VOD</t>
   </si>
@@ -335,6 +335,27 @@
   </si>
   <si>
     <t>FY17</t>
+  </si>
+  <si>
+    <t>(Projected)</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Service Revenue</t>
+  </si>
+  <si>
+    <t>Equipment Revenue</t>
+  </si>
+  <si>
+    <t>Customer Contracts Revenue</t>
+  </si>
+  <si>
+    <t>Other Revenue</t>
+  </si>
+  <si>
+    <t>Interest Revenue</t>
   </si>
 </sst>
 </file>
@@ -345,7 +366,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,8 +443,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +499,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,6 +731,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -696,24 +750,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,6 +760,32 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -821,7 +883,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -871,7 +933,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>114</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1214,7 +1276,7 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:D28"/>
+      <selection activeCell="H25" sqref="H25:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1234,31 +1296,31 @@
       <c r="F3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="G5" s="53" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="G5" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="55"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="59"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>1.0247999999999999</v>
+        <v>1.0459000000000001</v>
       </c>
       <c r="D6" s="7"/>
       <c r="G6" s="22">
@@ -1306,7 +1368,7 @@
       </c>
       <c r="C8" s="15">
         <f>C6*C7</f>
-        <v>29731.497599999999</v>
+        <v>30343.650800000003</v>
       </c>
       <c r="D8" s="7"/>
       <c r="G8" s="20"/>
@@ -1326,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="15">
-        <f>'Financial Model'!U72*Main!$C$13</f>
+        <f>'Financial Model'!U77*Main!$C$13</f>
         <v>6596.4800000000005</v>
       </c>
       <c r="D9" s="7" t="str">
@@ -1350,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="15">
-        <f>'Financial Model'!U73*Main!$C$13</f>
+        <f>'Financial Model'!U78*Main!$C$13</f>
         <v>62115.68</v>
       </c>
       <c r="D10" s="7" t="str">
@@ -1399,7 +1461,7 @@
       </c>
       <c r="C12" s="16">
         <f>C8-C11</f>
-        <v>85250.6976</v>
+        <v>85862.8508</v>
       </c>
       <c r="D12" s="8"/>
       <c r="G12" s="20"/>
@@ -1448,11 +1510,11 @@
       <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
       <c r="G15" s="20"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -1472,10 +1534,10 @@
       <c r="B16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="57"/>
+      <c r="D16" s="54"/>
       <c r="G16" s="20"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -1495,10 +1557,10 @@
       <c r="B17" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="57"/>
+      <c r="D17" s="54"/>
       <c r="G17" s="20"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
@@ -1515,10 +1577,10 @@
       <c r="B18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="57"/>
+      <c r="D18" s="54"/>
       <c r="G18" s="20"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -1533,8 +1595,8 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" s="18"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
       <c r="G19" s="20"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1574,11 +1636,11 @@
       <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
       <c r="G22" s="20"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -1595,10 +1657,10 @@
       <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="57"/>
+      <c r="D23" s="54"/>
       <c r="G23" s="20"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -1615,10 +1677,10 @@
       <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="56">
+      <c r="C24" s="53">
         <v>1984</v>
       </c>
-      <c r="D24" s="57"/>
+      <c r="D24" s="54"/>
       <c r="G24" s="20"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -1635,11 +1697,11 @@
       <c r="B25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="62">
-        <f>'Financial Model'!U42</f>
-        <v>836</v>
-      </c>
-      <c r="D25" s="57"/>
+      <c r="C25" s="60">
+        <f>'Financial Model'!U47*C13</f>
+        <v>735.68</v>
+      </c>
+      <c r="D25" s="54"/>
       <c r="G25" s="20"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -1654,8 +1716,8 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
       <c r="G26" s="20"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -1694,10 +1756,10 @@
       <c r="B28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="64"/>
       <c r="G28" s="20"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -1737,11 +1799,11 @@
       <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
+      <c r="B31" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
       <c r="G31" s="20"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
@@ -1758,11 +1820,11 @@
       <c r="B32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="60">
-        <f>C6/'Financial Model'!U67</f>
-        <v>0.52181577829650561</v>
-      </c>
-      <c r="D32" s="61"/>
+      <c r="C32" s="55">
+        <f>C6/'Financial Model'!U72</f>
+        <v>0.53255964336486661</v>
+      </c>
+      <c r="D32" s="56"/>
       <c r="G32" s="20"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -1779,8 +1841,8 @@
       <c r="B33" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="57"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
       <c r="G33" s="20"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -1797,11 +1859,11 @@
       <c r="B34" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="60">
-        <f>C6/'Financial Model'!U20</f>
-        <v>11.330601219512195</v>
-      </c>
-      <c r="D34" s="61"/>
+      <c r="C34" s="55">
+        <f>C6/'Financial Model'!U25</f>
+        <v>11.56389131097561</v>
+      </c>
+      <c r="D34" s="56"/>
       <c r="G34" s="21"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -1816,6 +1878,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="B5:D5"/>
@@ -1828,11 +1895,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C32:D32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28:D28" r:id="rId1" display="Link" xr:uid="{D050E430-21A3-4017-A567-1BB4BBA21237}"/>
@@ -1844,19 +1906,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18E1F45-FFBB-48B1-8EBD-5856C0E1925C}">
-  <dimension ref="A1:AA85"/>
+  <dimension ref="A1:AA90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R83" sqref="P83:R85"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="9.140625" style="26"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -1867,7 +1929,9 @@
     <col min="10" max="10" width="9.140625" style="26"/>
     <col min="11" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="9.140625" style="26"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="9.140625" style="65"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -1925,7 +1989,7 @@
       <c r="U1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="66" t="s">
         <v>45</v>
       </c>
       <c r="W1" s="24" t="s">
@@ -1969,6 +2033,9 @@
       <c r="U2" s="31">
         <v>44651</v>
       </c>
+      <c r="V2" s="67" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="3" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="27"/>
@@ -1986,1734 +2053,1944 @@
       <c r="U3" s="30">
         <v>44708</v>
       </c>
-    </row>
-    <row r="4" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+      <c r="V3" s="67"/>
+    </row>
+    <row r="4" spans="2:27" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="P4" s="42">
+        <v>42987</v>
+      </c>
+      <c r="Q4" s="42">
+        <v>41066</v>
+      </c>
+      <c r="R4" s="42">
+        <v>36458</v>
+      </c>
+      <c r="S4" s="42">
+        <v>37871</v>
+      </c>
+      <c r="T4" s="42">
+        <v>37141</v>
+      </c>
+      <c r="U4" s="42">
+        <v>38203</v>
+      </c>
+      <c r="V4" s="71"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+    </row>
+    <row r="5" spans="2:27" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="P5" s="42">
+        <v>4644</v>
+      </c>
+      <c r="Q5" s="42">
+        <v>5505</v>
+      </c>
+      <c r="R5" s="42">
+        <v>7208</v>
+      </c>
+      <c r="S5" s="42">
+        <v>7103</v>
+      </c>
+      <c r="T5" s="42">
+        <v>4824</v>
+      </c>
+      <c r="U5" s="42">
+        <v>5287</v>
+      </c>
+      <c r="V5" s="71"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="72"/>
+    </row>
+    <row r="6" spans="2:27" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="P6" s="42">
+        <v>47631</v>
+      </c>
+      <c r="Q6" s="42">
+        <v>46571</v>
+      </c>
+      <c r="R6" s="42">
+        <v>43666</v>
+      </c>
+      <c r="S6" s="42">
+        <v>44974</v>
+      </c>
+      <c r="T6" s="42">
+        <v>41965</v>
+      </c>
+      <c r="U6" s="42">
+        <v>43490</v>
+      </c>
+      <c r="V6" s="71"/>
+      <c r="W6" s="72"/>
+      <c r="X6" s="72"/>
+      <c r="Y6" s="72"/>
+    </row>
+    <row r="7" spans="2:27" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="75" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="P7" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="42">
+        <v>0</v>
+      </c>
+      <c r="R7" s="42">
+        <v>0</v>
+      </c>
+      <c r="S7" s="42">
+        <v>0</v>
+      </c>
+      <c r="T7" s="42">
+        <v>1694</v>
+      </c>
+      <c r="U7" s="42">
+        <v>1958</v>
+      </c>
+      <c r="V7" s="71"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="72"/>
+      <c r="Y7" s="72"/>
+    </row>
+    <row r="8" spans="2:27" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="P8" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="42">
+        <v>0</v>
+      </c>
+      <c r="R8" s="42">
+        <v>0</v>
+      </c>
+      <c r="S8" s="42">
+        <v>0</v>
+      </c>
+      <c r="T8" s="42">
+        <v>150</v>
+      </c>
+      <c r="U8" s="42">
+        <v>132</v>
+      </c>
+      <c r="V8" s="71"/>
+      <c r="W8" s="72"/>
+      <c r="X8" s="72"/>
+      <c r="Y8" s="72"/>
+    </row>
+    <row r="9" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="P4" s="34">
+      <c r="D9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="P9" s="34">
         <v>47631</v>
       </c>
-      <c r="Q4" s="34">
+      <c r="Q9" s="34">
         <v>46571</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R9" s="34">
         <v>43666</v>
       </c>
-      <c r="S4" s="34">
+      <c r="S9" s="34">
         <v>44974</v>
       </c>
-      <c r="T4" s="34">
+      <c r="T9" s="34">
         <v>43809</v>
       </c>
-      <c r="U4" s="34">
+      <c r="U9" s="34">
         <v>45580</v>
       </c>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
+      <c r="V9" s="68">
+        <f>U9*1.04</f>
+        <v>47403.200000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="35">
+      <c r="P10" s="35">
         <v>34576</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q10" s="35">
         <v>32771</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R10" s="35">
         <v>30160</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S10" s="35">
         <v>30682</v>
       </c>
-      <c r="T5" s="35">
+      <c r="T10" s="35">
         <v>30086</v>
       </c>
-      <c r="U5" s="35">
+      <c r="U10" s="35">
         <v>30574</v>
       </c>
-    </row>
-    <row r="6" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="V10" s="71">
+        <f>U10*1.02</f>
+        <v>31185.48</v>
+      </c>
+      <c r="W10" s="38"/>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+    </row>
+    <row r="11" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="P6" s="34">
-        <f t="shared" ref="P6:Q6" si="0">P4-P5</f>
+      <c r="D11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="P11" s="34">
+        <f t="shared" ref="P11:Q11" si="0">P9-P10</f>
         <v>13055</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q11" s="34">
         <f t="shared" si="0"/>
         <v>13800</v>
       </c>
-      <c r="R6" s="34">
-        <f>R4-R5</f>
+      <c r="R11" s="34">
+        <f>R9-R10</f>
         <v>13506</v>
       </c>
-      <c r="S6" s="34">
-        <f>S4-S5</f>
+      <c r="S11" s="34">
+        <f>S9-S10</f>
         <v>14292</v>
       </c>
-      <c r="T6" s="34">
-        <f>T4-T5</f>
+      <c r="T11" s="34">
+        <f>T9-T10</f>
         <v>13723</v>
       </c>
-      <c r="U6" s="34">
-        <f>U4-U5</f>
+      <c r="U11" s="34">
+        <f>U9-U10</f>
         <v>15006</v>
       </c>
-    </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="P7" s="35">
-        <v>4349</v>
-      </c>
-      <c r="Q7" s="35">
-        <v>4011</v>
-      </c>
-      <c r="R7" s="35">
-        <v>3891</v>
-      </c>
-      <c r="S7" s="35">
-        <v>3814</v>
-      </c>
-      <c r="T7" s="35">
-        <v>3522</v>
-      </c>
-      <c r="U7" s="35">
-        <v>3358</v>
-      </c>
-    </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P8" s="35">
-        <v>6080</v>
-      </c>
-      <c r="Q8" s="35">
-        <v>5644</v>
-      </c>
-      <c r="R8" s="35">
-        <v>5410</v>
-      </c>
-      <c r="S8" s="35">
-        <v>5810</v>
-      </c>
-      <c r="T8" s="35">
-        <v>5350</v>
-      </c>
-      <c r="U8" s="35">
-        <v>5713</v>
-      </c>
-    </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P9" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="35">
-        <v>0</v>
-      </c>
-      <c r="R9" s="35">
-        <v>575</v>
-      </c>
-      <c r="S9" s="35">
-        <v>660</v>
-      </c>
-      <c r="T9" s="35">
-        <v>664</v>
-      </c>
-      <c r="U9" s="35">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P10" s="35">
-        <v>47</v>
-      </c>
-      <c r="Q10" s="35">
-        <v>-59</v>
-      </c>
-      <c r="R10" s="35">
-        <v>-908</v>
-      </c>
-      <c r="S10" s="35">
-        <v>-2505</v>
-      </c>
-      <c r="T10" s="35">
-        <v>342</v>
-      </c>
-      <c r="U10" s="35">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P11" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="35">
-        <v>0</v>
-      </c>
-      <c r="R11" s="35">
-        <v>3525</v>
-      </c>
-      <c r="S11" s="35">
-        <v>1685</v>
-      </c>
-      <c r="T11" s="35">
-        <v>0</v>
-      </c>
-      <c r="U11" s="35">
-        <v>0</v>
+      <c r="V11" s="68">
+        <f>V9-V10</f>
+        <v>16217.720000000005</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="35">
+        <v>4349</v>
+      </c>
+      <c r="Q12" s="35">
+        <v>4011</v>
+      </c>
+      <c r="R12" s="35">
+        <v>3891</v>
+      </c>
+      <c r="S12" s="35">
+        <v>3814</v>
+      </c>
+      <c r="T12" s="35">
+        <v>3522</v>
+      </c>
+      <c r="U12" s="35">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="35">
+        <v>6080</v>
+      </c>
+      <c r="Q13" s="35">
+        <v>5644</v>
+      </c>
+      <c r="R13" s="35">
+        <v>5410</v>
+      </c>
+      <c r="S13" s="35">
+        <v>5810</v>
+      </c>
+      <c r="T13" s="35">
+        <v>5350</v>
+      </c>
+      <c r="U13" s="35">
+        <v>5713</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="35">
+        <v>0</v>
+      </c>
+      <c r="R14" s="35">
+        <v>575</v>
+      </c>
+      <c r="S14" s="35">
+        <v>660</v>
+      </c>
+      <c r="T14" s="35">
+        <v>664</v>
+      </c>
+      <c r="U14" s="35">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15" s="35">
+        <v>47</v>
+      </c>
+      <c r="Q15" s="35">
+        <v>-59</v>
+      </c>
+      <c r="R15" s="35">
+        <v>-908</v>
+      </c>
+      <c r="S15" s="35">
+        <v>-2505</v>
+      </c>
+      <c r="T15" s="35">
+        <v>342</v>
+      </c>
+      <c r="U15" s="35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P16" s="35">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>0</v>
+      </c>
+      <c r="R16" s="35">
+        <v>3525</v>
+      </c>
+      <c r="S16" s="35">
+        <v>1685</v>
+      </c>
+      <c r="T16" s="35">
+        <v>0</v>
+      </c>
+      <c r="U16" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="35">
+      <c r="P17" s="35">
         <v>1052</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q17" s="35">
         <v>213</v>
       </c>
-      <c r="R12" s="35">
+      <c r="R17" s="35">
         <v>-148</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S17" s="35">
         <v>4281</v>
       </c>
-      <c r="T12" s="35">
+      <c r="T17" s="35">
         <v>568</v>
       </c>
-      <c r="U12" s="35">
+      <c r="U17" s="35">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+    <row r="18" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="P13" s="34">
-        <f t="shared" ref="P13:Q13" si="1">P6-P7-P8-P9+P10-P11+P12</f>
+      <c r="D18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="P18" s="34">
+        <f t="shared" ref="P18:Q18" si="1">P11-P12-P13-P14+P15-P16+P17</f>
         <v>3725</v>
       </c>
-      <c r="Q13" s="34">
+      <c r="Q18" s="34">
         <f t="shared" si="1"/>
         <v>4299</v>
       </c>
-      <c r="R13" s="34">
-        <f>R6-R7-R8-R9+R10-R11+R12</f>
+      <c r="R18" s="34">
+        <f>R11-R12-R13-R14+R15-R16+R17</f>
         <v>-951</v>
       </c>
-      <c r="S13" s="34">
-        <f>S6-S7-S8-S9+S10-S11+S12</f>
+      <c r="S18" s="34">
+        <f>S11-S12-S13-S14+S15-S16+S17</f>
         <v>4099</v>
       </c>
-      <c r="T13" s="34">
-        <f>T6-T7-T8-T9+T10-T11+T12</f>
+      <c r="T18" s="34">
+        <f>T11-T12-T13-T14+T15-T16+T17</f>
         <v>5097</v>
       </c>
-      <c r="U13" s="34">
-        <f>U6-U7-U8-U9+U10-U11+U12</f>
+      <c r="U18" s="34">
+        <f>U11-U12-U13-U14+U15-U16+U17</f>
         <v>5664</v>
       </c>
-    </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+      <c r="V18" s="69"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P14" s="35">
+      <c r="P19" s="35">
         <v>1</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q19" s="35">
         <v>32</v>
       </c>
-      <c r="R14" s="35">
+      <c r="R19" s="35">
         <v>7</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S19" s="35">
         <v>3</v>
       </c>
-      <c r="T14" s="35">
+      <c r="T19" s="35">
         <v>0</v>
       </c>
-      <c r="U14" s="35">
+      <c r="U19" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="35">
+      <c r="P20" s="35">
         <v>474</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q20" s="35">
         <v>685</v>
       </c>
-      <c r="R15" s="35">
+      <c r="R20" s="35">
         <v>433</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S20" s="35">
         <v>248</v>
       </c>
-      <c r="T15" s="35">
+      <c r="T20" s="35">
         <v>330</v>
       </c>
-      <c r="U15" s="35">
+      <c r="U20" s="35">
         <v>254</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P16" s="35">
+      <c r="P21" s="35">
         <v>1406</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q21" s="35">
         <v>1074</v>
       </c>
-      <c r="R16" s="35">
+      <c r="R21" s="35">
         <v>2088</v>
       </c>
-      <c r="S16" s="35">
+      <c r="S21" s="35">
         <v>3549</v>
       </c>
-      <c r="T16" s="35">
+      <c r="T21" s="35">
         <v>1027</v>
       </c>
-      <c r="U16" s="35">
+      <c r="U21" s="35">
         <v>1964</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P17" s="35">
-        <f t="shared" ref="P17:Q17" si="2">P13-P14+P15-P16</f>
+      <c r="P22" s="35">
+        <f t="shared" ref="P22:Q22" si="2">P18-P19+P20-P21</f>
         <v>2792</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q22" s="35">
         <f t="shared" si="2"/>
         <v>3878</v>
       </c>
-      <c r="R17" s="35">
-        <f>R13-R14+R15-R16</f>
+      <c r="R22" s="35">
+        <f>R18-R19+R20-R21</f>
         <v>-2613</v>
       </c>
-      <c r="S17" s="35">
-        <f>S13-S14+S15-S16</f>
+      <c r="S22" s="35">
+        <f>S18-S19+S20-S21</f>
         <v>795</v>
       </c>
-      <c r="T17" s="35">
-        <f>T13-T14+T15-T16</f>
+      <c r="T22" s="35">
+        <f>T18-T19+T20-T21</f>
         <v>4400</v>
       </c>
-      <c r="U17" s="35">
-        <f>U13-U14+U15-U16</f>
+      <c r="U22" s="35">
+        <f>U18-U19+U20-U21</f>
         <v>3954</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P18" s="35">
+      <c r="P23" s="35">
         <v>4764</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q23" s="35">
         <v>-879</v>
       </c>
-      <c r="R18" s="35">
+      <c r="R23" s="35">
         <v>1496</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S23" s="35">
         <v>1250</v>
       </c>
-      <c r="T18" s="35">
+      <c r="T23" s="35">
         <v>3864</v>
       </c>
-      <c r="U18" s="35">
+      <c r="U23" s="35">
         <v>1330</v>
       </c>
     </row>
-    <row r="19" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+    <row r="24" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="P19" s="34">
-        <f t="shared" ref="P19:Q19" si="3">P17-P18</f>
+      <c r="D24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="P24" s="34">
+        <f t="shared" ref="P24:Q24" si="3">P22-P23</f>
         <v>-1972</v>
       </c>
-      <c r="Q19" s="34">
+      <c r="Q24" s="34">
         <f t="shared" si="3"/>
         <v>4757</v>
       </c>
-      <c r="R19" s="34">
-        <f>R17-R18</f>
+      <c r="R24" s="34">
+        <f>R22-R23</f>
         <v>-4109</v>
       </c>
-      <c r="S19" s="34">
-        <f>S17-S18</f>
+      <c r="S24" s="34">
+        <f>S22-S23</f>
         <v>-455</v>
       </c>
-      <c r="T19" s="34">
-        <f>T17-T18</f>
+      <c r="T24" s="34">
+        <f>T22-T23</f>
         <v>536</v>
       </c>
-      <c r="U19" s="34">
-        <f>U17-U18</f>
+      <c r="U24" s="34">
+        <f>U22-U23</f>
         <v>2624</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
+      <c r="V24" s="69"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P20" s="1">
-        <f t="shared" ref="P20:R20" si="4">P19/P21</f>
+      <c r="P25" s="1">
+        <f t="shared" ref="P25:R25" si="4">P24/P26</f>
         <v>-7.0501590933466807E-2</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q25" s="1">
         <f t="shared" si="4"/>
         <v>0.17129996398991718</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R25" s="1">
         <f t="shared" si="4"/>
         <v>-0.14883906255659796</v>
       </c>
-      <c r="S20" s="1">
-        <f t="shared" ref="S20" si="5">S19/S21</f>
+      <c r="S25" s="1">
+        <f t="shared" ref="S25" si="5">S24/S26</f>
         <v>-1.5454113171659534E-2</v>
       </c>
-      <c r="T20" s="1">
-        <f t="shared" ref="T20" si="6">T19/T21</f>
+      <c r="T25" s="1">
+        <f t="shared" ref="T25" si="6">T24/T26</f>
         <v>1.8113003514463367E-2</v>
       </c>
-      <c r="U20" s="1">
-        <f>U19/U21</f>
+      <c r="U25" s="1">
+        <f>U24/U26</f>
         <v>9.0445332965669381E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P26" s="35">
         <v>27971</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q26" s="35">
         <v>27770</v>
       </c>
-      <c r="R21" s="35">
+      <c r="R26" s="35">
         <v>27607</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S26" s="35">
         <v>29442</v>
       </c>
-      <c r="T21" s="35">
+      <c r="T26" s="35">
         <v>29592</v>
       </c>
-      <c r="U21" s="35">
+      <c r="U26" s="35">
         <v>29012</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
+      <c r="V26" s="71">
+        <f>U26</f>
+        <v>29012</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="Q23" s="37">
-        <f t="shared" ref="Q23" si="7">Q4/P4-1</f>
+      <c r="D28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="Q28" s="37">
+        <f t="shared" ref="Q28" si="7">Q9/P9-1</f>
         <v>-2.2254414142050316E-2</v>
       </c>
-      <c r="R23" s="37">
-        <f t="shared" ref="R23" si="8">R4/Q4-1</f>
+      <c r="R28" s="37">
+        <f t="shared" ref="R28" si="8">R9/Q9-1</f>
         <v>-6.2377874643018139E-2</v>
       </c>
-      <c r="S23" s="37">
-        <f t="shared" ref="S23:T23" si="9">S4/R4-1</f>
+      <c r="S28" s="37">
+        <f t="shared" ref="S28:T28" si="9">S9/R9-1</f>
         <v>2.9954655796271767E-2</v>
       </c>
-      <c r="T23" s="37">
+      <c r="T28" s="37">
         <f t="shared" si="9"/>
         <v>-2.5903855560990841E-2</v>
       </c>
-      <c r="U23" s="37">
-        <f>U4/T4-1</f>
+      <c r="U28" s="37">
+        <f>U9/T9-1</f>
         <v>4.0425483348170532E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="V28" s="74">
+        <f>V9/U9-1</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P26" s="38">
-        <f t="shared" ref="P26:Q26" si="10">P6/P4</f>
+      <c r="P31" s="38">
+        <f t="shared" ref="P31" si="10">P11/P9</f>
         <v>0.27408620436270498</v>
       </c>
-      <c r="Q26" s="38">
-        <f t="shared" ref="Q26:R26" si="11">Q6/Q4</f>
+      <c r="Q31" s="38">
+        <f t="shared" ref="Q31" si="11">Q11/Q9</f>
         <v>0.29632174529213456</v>
       </c>
-      <c r="R26" s="38">
-        <f t="shared" ref="R26:S26" si="12">R6/R4</f>
+      <c r="R31" s="38">
+        <f t="shared" ref="R31:S31" si="12">R11/R9</f>
         <v>0.30930243209819996</v>
       </c>
-      <c r="S26" s="38">
+      <c r="S31" s="38">
         <f t="shared" si="12"/>
         <v>0.31778360830702185</v>
       </c>
-      <c r="T26" s="38">
-        <f t="shared" ref="T26" si="13">T6/T4</f>
+      <c r="T31" s="38">
+        <f t="shared" ref="T31" si="13">T11/T9</f>
         <v>0.31324613663859024</v>
       </c>
-      <c r="U26" s="38">
-        <f>U6/U4</f>
+      <c r="U31" s="38">
+        <f>U11/U9</f>
         <v>0.32922334357174199</v>
       </c>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+      <c r="V31" s="73">
+        <f t="shared" ref="V31" si="14">V11/V9</f>
+        <v>0.34212289465690088</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="P27" s="38">
-        <f t="shared" ref="P27:Q27" si="14">P13/P4</f>
+      <c r="P32" s="38">
+        <f t="shared" ref="P32" si="15">P18/P9</f>
         <v>7.8205370452016545E-2</v>
       </c>
-      <c r="Q27" s="38">
-        <f t="shared" ref="Q27:R27" si="15">Q13/Q4</f>
+      <c r="Q32" s="38">
+        <f t="shared" ref="Q32" si="16">Q18/Q9</f>
         <v>9.2310665435571496E-2</v>
       </c>
-      <c r="R27" s="38">
-        <f t="shared" ref="R27:S27" si="16">R13/R4</f>
+      <c r="R32" s="38">
+        <f t="shared" ref="R32:S32" si="17">R18/R9</f>
         <v>-2.177895845738103E-2</v>
       </c>
-      <c r="S27" s="38">
-        <f t="shared" si="16"/>
+      <c r="S32" s="38">
+        <f t="shared" si="17"/>
         <v>9.1141548450215687E-2</v>
       </c>
-      <c r="T27" s="38">
-        <f t="shared" ref="T27" si="17">T13/T4</f>
+      <c r="T32" s="38">
+        <f t="shared" ref="T32" si="18">T18/T9</f>
         <v>0.11634595631034719</v>
       </c>
-      <c r="U27" s="38">
-        <f>U13/U4</f>
+      <c r="U32" s="38">
+        <f>U18/U9</f>
         <v>0.12426502852128127</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+      <c r="V32" s="73">
+        <f t="shared" ref="V32" si="19">V18/V9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P28" s="38">
-        <f t="shared" ref="P28:Q28" si="18">P19/P4</f>
+      <c r="P33" s="38">
+        <f t="shared" ref="P33" si="20">P24/P9</f>
         <v>-4.1401608196342719E-2</v>
       </c>
-      <c r="Q28" s="38">
-        <f t="shared" ref="Q28:R28" si="19">Q19/Q4</f>
+      <c r="Q33" s="38">
+        <f t="shared" ref="Q33" si="21">Q24/Q9</f>
         <v>0.10214511176483219</v>
       </c>
-      <c r="R28" s="38">
-        <f t="shared" ref="R28:S28" si="20">R19/R4</f>
+      <c r="R33" s="38">
+        <f t="shared" ref="R33:S33" si="22">R24/R9</f>
         <v>-9.4100673292722023E-2</v>
       </c>
-      <c r="S28" s="38">
-        <f t="shared" si="20"/>
+      <c r="S33" s="38">
+        <f t="shared" si="22"/>
         <v>-1.0116956463734603E-2</v>
       </c>
-      <c r="T28" s="38">
-        <f t="shared" ref="T28" si="21">T19/T4</f>
+      <c r="T33" s="38">
+        <f t="shared" ref="T33" si="23">T24/T9</f>
         <v>1.2234928895888973E-2</v>
       </c>
-      <c r="U28" s="38">
-        <f>U19/U4</f>
+      <c r="U33" s="38">
+        <f>U24/U9</f>
         <v>5.7569109258446688E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+      <c r="V33" s="73">
+        <f t="shared" ref="V33" si="24">V24/V9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P29" s="38">
-        <f t="shared" ref="P29:Q29" si="22">P19/P4</f>
+      <c r="P34" s="38">
+        <f t="shared" ref="P34" si="25">P24/P9</f>
         <v>-4.1401608196342719E-2</v>
       </c>
-      <c r="Q29" s="38">
-        <f t="shared" ref="Q29:R29" si="23">Q19/Q4</f>
+      <c r="Q34" s="38">
+        <f t="shared" ref="Q34" si="26">Q24/Q9</f>
         <v>0.10214511176483219</v>
       </c>
-      <c r="R29" s="38">
-        <f t="shared" ref="R29:S29" si="24">R19/R4</f>
+      <c r="R34" s="38">
+        <f t="shared" ref="R34:S34" si="27">R24/R9</f>
         <v>-9.4100673292722023E-2</v>
       </c>
-      <c r="S29" s="38">
-        <f t="shared" si="24"/>
+      <c r="S34" s="38">
+        <f t="shared" si="27"/>
         <v>-1.0116956463734603E-2</v>
       </c>
-      <c r="T29" s="38">
-        <f t="shared" ref="T29" si="25">T19/T4</f>
+      <c r="T34" s="38">
+        <f t="shared" ref="T34" si="28">T24/T9</f>
         <v>1.2234928895888973E-2</v>
       </c>
-      <c r="U29" s="38">
-        <f>U19/U4</f>
+      <c r="U34" s="38">
+        <f>U24/U9</f>
         <v>5.7569109258446688E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B33" s="39" t="s">
+      <c r="V34" s="73">
+        <f t="shared" ref="V34" si="29">V24/V9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B38" s="39" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="P34" s="35">
+      <c r="P39" s="35">
         <f>26808+19412</f>
         <v>46220</v>
       </c>
-      <c r="Q34" s="35">
+      <c r="Q39" s="35">
         <f>26734+16523</f>
         <v>43257</v>
       </c>
-      <c r="R34" s="35">
+      <c r="R39" s="35">
         <f>23353+17652</f>
         <v>41005</v>
       </c>
-      <c r="S34" s="35">
+      <c r="S39" s="35">
         <f>31271+22252</f>
         <v>53523</v>
       </c>
-      <c r="T34" s="35">
+      <c r="T39" s="35">
         <f>31731+21818</f>
         <v>53549</v>
       </c>
-      <c r="U34" s="35">
+      <c r="U39" s="35">
         <f>31884+21360</f>
         <v>53244</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P35" s="35">
+      <c r="P40" s="35">
         <v>30204</v>
       </c>
-      <c r="Q35" s="35">
+      <c r="Q40" s="35">
         <v>28325</v>
       </c>
-      <c r="R35" s="35">
+      <c r="R40" s="35">
         <v>27432</v>
       </c>
-      <c r="S35" s="35">
+      <c r="S40" s="35">
         <v>39197</v>
       </c>
-      <c r="T35" s="35">
+      <c r="T40" s="35">
         <v>41243</v>
       </c>
-      <c r="U35" s="35">
+      <c r="U40" s="35">
         <v>40804</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="P36" s="35">
+      <c r="P41" s="35">
         <v>3138</v>
       </c>
-      <c r="Q36" s="35">
+      <c r="Q41" s="35">
         <v>2538</v>
       </c>
-      <c r="R36" s="35">
+      <c r="R41" s="35">
         <v>3952</v>
       </c>
-      <c r="S36" s="35">
+      <c r="S41" s="35">
         <v>5831</v>
       </c>
-      <c r="T36" s="35">
+      <c r="T41" s="35">
         <v>4670</v>
       </c>
-      <c r="U36" s="35">
+      <c r="U41" s="35">
         <v>4268</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P37" s="35">
+      <c r="P42" s="35">
         <v>3459</v>
       </c>
-      <c r="Q37" s="35">
+      <c r="Q42" s="35">
         <v>3204</v>
       </c>
-      <c r="R37" s="35">
+      <c r="R42" s="35">
         <v>870</v>
       </c>
-      <c r="S37" s="35">
+      <c r="S42" s="35">
         <v>792</v>
       </c>
-      <c r="T37" s="35">
+      <c r="T42" s="35">
         <v>925</v>
       </c>
-      <c r="U37" s="35">
+      <c r="U42" s="35">
         <v>1073</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P38" s="35">
+      <c r="P43" s="35">
         <v>24300</v>
       </c>
-      <c r="Q38" s="35">
+      <c r="Q43" s="35">
         <v>26200</v>
       </c>
-      <c r="R38" s="35">
+      <c r="R43" s="35">
         <v>24753</v>
       </c>
-      <c r="S38" s="35">
+      <c r="S43" s="35">
         <v>23606</v>
       </c>
-      <c r="T38" s="35">
+      <c r="T43" s="35">
         <v>21569</v>
       </c>
-      <c r="U38" s="35">
+      <c r="U43" s="35">
         <v>19089</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P39" s="35">
+      <c r="P44" s="35">
         <v>57</v>
       </c>
-      <c r="Q39" s="35">
+      <c r="Q44" s="35">
         <v>110</v>
       </c>
-      <c r="R39" s="35">
+      <c r="R44" s="35">
         <v>94</v>
       </c>
-      <c r="S39" s="35">
+      <c r="S44" s="35">
         <v>590</v>
       </c>
-      <c r="T39" s="35">
+      <c r="T44" s="35">
         <v>60</v>
       </c>
-      <c r="U39" s="35">
+      <c r="U44" s="35">
         <v>555</v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P40" s="35">
+      <c r="P45" s="35">
         <v>4569</v>
       </c>
-      <c r="Q40" s="35">
+      <c r="Q45" s="35">
         <v>4026</v>
       </c>
-      <c r="R40" s="35">
+      <c r="R45" s="35">
         <v>5170</v>
       </c>
-      <c r="S40" s="35">
+      <c r="S45" s="35">
         <v>10378</v>
       </c>
-      <c r="T40" s="35">
+      <c r="T45" s="35">
         <v>4777</v>
       </c>
-      <c r="U40" s="35">
+      <c r="U45" s="35">
         <v>6383</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P41" s="35">
-        <f>SUM(P34:P40)</f>
+      <c r="P46" s="35">
+        <f t="shared" ref="P46:U46" si="30">SUM(P39:P45)</f>
         <v>111947</v>
       </c>
-      <c r="Q41" s="35">
-        <f>SUM(Q34:Q40)</f>
+      <c r="Q46" s="35">
+        <f t="shared" si="30"/>
         <v>107660</v>
       </c>
-      <c r="R41" s="35">
-        <f>SUM(R34:R40)</f>
+      <c r="R46" s="35">
+        <f t="shared" si="30"/>
         <v>103276</v>
       </c>
-      <c r="S41" s="35">
-        <f>SUM(S34:S40)</f>
+      <c r="S46" s="35">
+        <f t="shared" si="30"/>
         <v>133917</v>
       </c>
-      <c r="T41" s="35">
-        <f>SUM(T34:T40)</f>
+      <c r="T46" s="35">
+        <f t="shared" si="30"/>
         <v>126793</v>
       </c>
-      <c r="U41" s="35">
-        <f>SUM(U34:U40)</f>
+      <c r="U46" s="35">
+        <f t="shared" si="30"/>
         <v>125416</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="2" t="s">
+    <row r="47" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="P42" s="34">
+      <c r="D47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="L47" s="32"/>
+      <c r="P47" s="34">
         <v>576</v>
       </c>
-      <c r="Q42" s="34">
+      <c r="Q47" s="34">
         <v>581</v>
       </c>
-      <c r="R42" s="34">
+      <c r="R47" s="34">
         <v>714</v>
       </c>
-      <c r="S42" s="34">
+      <c r="S47" s="34">
         <v>585</v>
       </c>
-      <c r="T42" s="34">
+      <c r="T47" s="34">
         <v>676</v>
       </c>
-      <c r="U42" s="34">
+      <c r="U47" s="34">
         <v>836</v>
       </c>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+      <c r="V47" s="69"/>
+    </row>
+    <row r="48" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P43" s="35">
+      <c r="P48" s="35">
         <v>150</v>
       </c>
-      <c r="Q43" s="35">
+      <c r="Q48" s="35">
         <v>106</v>
       </c>
-      <c r="R43" s="35">
+      <c r="R48" s="35">
         <v>264</v>
       </c>
-      <c r="S43" s="35">
+      <c r="S48" s="35">
         <v>275</v>
       </c>
-      <c r="T43" s="35">
+      <c r="T48" s="35">
         <v>434</v>
       </c>
-      <c r="U43" s="35">
+      <c r="U48" s="35">
         <v>296</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+    <row r="49" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="P44" s="35">
+      <c r="P49" s="35">
         <v>9861</v>
       </c>
-      <c r="Q44" s="35">
+      <c r="Q49" s="35">
         <v>9975</v>
       </c>
-      <c r="R44" s="35">
+      <c r="R49" s="35">
         <v>12190</v>
       </c>
-      <c r="S44" s="35">
+      <c r="S49" s="35">
         <v>11411</v>
       </c>
-      <c r="T44" s="35">
+      <c r="T49" s="35">
         <v>10923</v>
       </c>
-      <c r="U44" s="35">
+      <c r="U49" s="35">
         <v>11019</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="50" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P45" s="35">
+      <c r="P50" s="35">
         <v>6120</v>
       </c>
-      <c r="Q45" s="35">
+      <c r="Q50" s="35">
         <v>8795</v>
       </c>
-      <c r="R45" s="35">
+      <c r="R50" s="35">
         <v>13012</v>
       </c>
-      <c r="S45" s="35">
+      <c r="S50" s="35">
         <v>7089</v>
       </c>
-      <c r="T45" s="35">
+      <c r="T50" s="35">
         <v>9159</v>
       </c>
-      <c r="U45" s="35">
+      <c r="U50" s="35">
         <v>7931</v>
       </c>
     </row>
-    <row r="46" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
+    <row r="51" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="P46" s="34">
+      <c r="D51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="P51" s="34">
         <v>8835</v>
       </c>
-      <c r="Q46" s="34">
+      <c r="Q51" s="34">
         <v>4674</v>
       </c>
-      <c r="R46" s="34">
+      <c r="R51" s="34">
         <v>13637</v>
       </c>
-      <c r="S46" s="34">
+      <c r="S51" s="34">
         <v>13284</v>
       </c>
-      <c r="T46" s="34">
+      <c r="T51" s="34">
         <v>5821</v>
       </c>
-      <c r="U46" s="34">
+      <c r="U51" s="34">
         <v>7496</v>
       </c>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+      <c r="V51" s="69"/>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P47" s="35">
+      <c r="P52" s="35">
         <v>17195</v>
       </c>
-      <c r="Q47" s="35">
+      <c r="Q52" s="35">
         <v>13820</v>
       </c>
-      <c r="R47" s="35">
+      <c r="R52" s="35">
         <v>-231</v>
       </c>
-      <c r="S47" s="35">
+      <c r="S52" s="35">
         <v>1607</v>
       </c>
-      <c r="T47" s="35">
+      <c r="T52" s="35">
         <v>1257</v>
       </c>
-      <c r="U47" s="35">
+      <c r="U52" s="35">
         <v>959</v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="53" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="P48" s="35">
-        <f>P41+SUM(P42:P47)</f>
+      <c r="P53" s="35">
+        <f t="shared" ref="P53:U53" si="31">P46+SUM(P47:P52)</f>
         <v>154684</v>
       </c>
-      <c r="Q48" s="35">
-        <f>Q41+SUM(Q42:Q47)</f>
+      <c r="Q53" s="35">
+        <f t="shared" si="31"/>
         <v>145611</v>
       </c>
-      <c r="R48" s="35">
-        <f>R41+SUM(R42:R47)</f>
+      <c r="R53" s="35">
+        <f t="shared" si="31"/>
         <v>142862</v>
       </c>
-      <c r="S48" s="35">
-        <f>S41+SUM(S42:S47)</f>
+      <c r="S53" s="35">
+        <f t="shared" si="31"/>
         <v>168168</v>
       </c>
-      <c r="T48" s="35">
-        <f>T41+SUM(T42:T47)</f>
+      <c r="T53" s="35">
+        <f t="shared" si="31"/>
         <v>155063</v>
       </c>
-      <c r="U48" s="35">
-        <f>U41+SUM(U42:U47)</f>
+      <c r="U53" s="35">
+        <f t="shared" si="31"/>
         <v>153953</v>
       </c>
     </row>
-    <row r="50" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="2" t="s">
+    <row r="55" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="P50" s="34">
+      <c r="D55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="L55" s="32"/>
+      <c r="P55" s="34">
         <v>34523</v>
       </c>
-      <c r="Q50" s="34">
+      <c r="Q55" s="34">
         <v>32908</v>
       </c>
-      <c r="R50" s="34">
+      <c r="R55" s="34">
         <v>48685</v>
       </c>
-      <c r="S50" s="34">
+      <c r="S55" s="34">
         <v>62892</v>
       </c>
-      <c r="T50" s="34">
+      <c r="T55" s="34">
         <v>59272</v>
       </c>
-      <c r="U50" s="34">
+      <c r="U55" s="34">
         <v>58131</v>
       </c>
-    </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
+      <c r="V55" s="69"/>
+    </row>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="P51" s="35">
+      <c r="P56" s="35">
         <v>535</v>
       </c>
-      <c r="Q51" s="35">
+      <c r="Q56" s="35">
         <v>644</v>
       </c>
-      <c r="R51" s="35">
+      <c r="R56" s="35">
         <v>478</v>
       </c>
-      <c r="S51" s="35">
+      <c r="S56" s="35">
         <v>2043</v>
       </c>
-      <c r="T51" s="35">
+      <c r="T56" s="35">
         <v>2095</v>
       </c>
-      <c r="U51" s="35">
+      <c r="U56" s="35">
         <v>520</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+    <row r="57" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P52" s="35">
+      <c r="P57" s="35">
         <v>651</v>
       </c>
-      <c r="Q52" s="35">
+      <c r="Q57" s="35">
         <v>520</v>
       </c>
-      <c r="R52" s="35">
+      <c r="R57" s="35">
         <v>551</v>
       </c>
-      <c r="S52" s="35">
+      <c r="S57" s="35">
         <v>438</v>
       </c>
-      <c r="T52" s="35">
+      <c r="T57" s="35">
         <v>513</v>
       </c>
-      <c r="U52" s="35">
+      <c r="U57" s="35">
         <v>281</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+    <row r="58" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P53" s="35">
+      <c r="P58" s="35">
         <v>1130</v>
       </c>
-      <c r="Q53" s="35">
+      <c r="Q58" s="35">
         <v>1065</v>
       </c>
-      <c r="R53" s="35">
+      <c r="R58" s="35">
         <v>1242</v>
       </c>
-      <c r="S53" s="35">
+      <c r="S58" s="35">
         <v>1474</v>
       </c>
-      <c r="T53" s="35">
+      <c r="T58" s="35">
         <v>1747</v>
       </c>
-      <c r="U53" s="35">
+      <c r="U58" s="35">
         <v>1881</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+    <row r="59" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="P54" s="35">
+      <c r="P59" s="35">
         <v>1737</v>
       </c>
-      <c r="Q54" s="35">
+      <c r="Q59" s="35">
         <v>2843</v>
       </c>
-      <c r="R54" s="35">
+      <c r="R59" s="35">
         <v>2938</v>
       </c>
-      <c r="S54" s="35">
+      <c r="S59" s="35">
         <v>5189</v>
       </c>
-      <c r="T54" s="35">
+      <c r="T59" s="35">
         <v>4909</v>
       </c>
-      <c r="U54" s="35">
+      <c r="U59" s="35">
         <v>2516</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+    <row r="60" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P55" s="35">
-        <f>SUM(P50:P54)</f>
+      <c r="P60" s="35">
+        <f t="shared" ref="P60:U60" si="32">SUM(P55:P59)</f>
         <v>38576</v>
       </c>
-      <c r="Q55" s="35">
-        <f>SUM(Q50:Q54)</f>
+      <c r="Q60" s="35">
+        <f t="shared" si="32"/>
         <v>37980</v>
       </c>
-      <c r="R55" s="35">
-        <f>SUM(R50:R54)</f>
+      <c r="R60" s="35">
+        <f t="shared" si="32"/>
         <v>53894</v>
       </c>
-      <c r="S55" s="35">
-        <f>SUM(S50:S54)</f>
+      <c r="S60" s="35">
+        <f t="shared" si="32"/>
         <v>72036</v>
       </c>
-      <c r="T55" s="35">
-        <f>SUM(T50:T54)</f>
+      <c r="T60" s="35">
+        <f t="shared" si="32"/>
         <v>68536</v>
       </c>
-      <c r="U55" s="35">
-        <f>SUM(U50:U54)</f>
+      <c r="U60" s="35">
+        <f t="shared" si="32"/>
         <v>63329</v>
       </c>
     </row>
-    <row r="56" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="2" t="s">
+    <row r="61" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="L56" s="32"/>
-      <c r="P56" s="34">
+      <c r="D61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="L61" s="32"/>
+      <c r="P61" s="34">
         <v>12051</v>
       </c>
-      <c r="Q56" s="34">
+      <c r="Q61" s="34">
         <v>10351</v>
       </c>
-      <c r="R56" s="34">
+      <c r="R61" s="34">
         <v>4270</v>
       </c>
-      <c r="S56" s="34">
+      <c r="S61" s="34">
         <v>11826</v>
       </c>
-      <c r="T56" s="34">
+      <c r="T61" s="34">
         <v>8488</v>
       </c>
-      <c r="U56" s="34">
+      <c r="U61" s="34">
         <v>11961</v>
       </c>
-    </row>
-    <row r="57" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="2" t="s">
+      <c r="V61" s="69"/>
+    </row>
+    <row r="62" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="P57" s="34">
+      <c r="D62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="L62" s="32"/>
+      <c r="P62" s="34">
         <v>0</v>
       </c>
-      <c r="Q57" s="34">
+      <c r="Q62" s="34">
         <v>0</v>
       </c>
-      <c r="R57" s="34">
+      <c r="R62" s="34">
         <v>1844</v>
       </c>
-      <c r="S57" s="34">
+      <c r="S62" s="34">
         <v>1850</v>
       </c>
-      <c r="T57" s="34">
+      <c r="T62" s="34">
         <v>492</v>
       </c>
-      <c r="U57" s="34">
+      <c r="U62" s="34">
         <v>494</v>
       </c>
-    </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+      <c r="V62" s="69"/>
+    </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P58" s="34">
+      <c r="P63" s="34">
         <v>661</v>
       </c>
-      <c r="Q58" s="35">
+      <c r="Q63" s="35">
         <v>541</v>
       </c>
-      <c r="R58" s="35">
+      <c r="R63" s="35">
         <v>596</v>
       </c>
-      <c r="S58" s="35">
+      <c r="S63" s="35">
         <v>671</v>
       </c>
-      <c r="T58" s="35">
+      <c r="T63" s="35">
         <v>769</v>
       </c>
-      <c r="U58" s="35">
+      <c r="U63" s="35">
         <v>864</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B59" s="1" t="s">
+    <row r="64" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P59" s="35">
+      <c r="P64" s="35">
         <v>1049</v>
       </c>
-      <c r="Q59" s="35">
+      <c r="Q64" s="35">
         <v>891</v>
       </c>
-      <c r="R59" s="35">
+      <c r="R64" s="35">
         <v>1160</v>
       </c>
-      <c r="S59" s="35">
+      <c r="S64" s="35">
         <v>1024</v>
       </c>
-      <c r="T59" s="35">
+      <c r="T64" s="35">
         <v>892</v>
       </c>
-      <c r="U59" s="35">
+      <c r="U64" s="35">
         <v>667</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="P60" s="35">
+      <c r="P65" s="35">
         <v>16834</v>
       </c>
-      <c r="Q60" s="35">
+      <c r="Q65" s="35">
         <v>16242</v>
       </c>
-      <c r="R60" s="35">
+      <c r="R65" s="35">
         <v>17653</v>
       </c>
-      <c r="S60" s="35">
+      <c r="S65" s="35">
         <v>17085</v>
       </c>
-      <c r="T60" s="35">
+      <c r="T65" s="35">
         <v>18070</v>
       </c>
-      <c r="U60" s="35">
+      <c r="U65" s="35">
         <v>19661</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="P61" s="35">
-        <f>P55+SUM(P56:P60)</f>
+      <c r="P66" s="35">
+        <f t="shared" ref="P66:U66" si="33">P60+SUM(P61:P65)</f>
         <v>69171</v>
       </c>
-      <c r="Q61" s="35">
-        <f>Q55+SUM(Q56:Q60)</f>
+      <c r="Q66" s="35">
+        <f t="shared" si="33"/>
         <v>66005</v>
       </c>
-      <c r="R61" s="35">
-        <f>R55+SUM(R56:R60)</f>
+      <c r="R66" s="35">
+        <f t="shared" si="33"/>
         <v>79417</v>
       </c>
-      <c r="S61" s="35">
-        <f>S55+SUM(S56:S60)</f>
+      <c r="S66" s="35">
+        <f t="shared" si="33"/>
         <v>104492</v>
       </c>
-      <c r="T61" s="35">
-        <f>T55+SUM(T56:T60)</f>
+      <c r="T66" s="35">
+        <f t="shared" si="33"/>
         <v>97247</v>
       </c>
-      <c r="U61" s="35">
-        <f>U55+SUM(U56:U60)</f>
+      <c r="U66" s="35">
+        <f t="shared" si="33"/>
         <v>96976</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="P63" s="35">
+      <c r="P68" s="35">
         <v>73719</v>
       </c>
-      <c r="Q63" s="35">
+      <c r="Q68" s="35">
         <v>68607</v>
       </c>
-      <c r="R63" s="35">
+      <c r="R68" s="35">
         <v>63445</v>
       </c>
-      <c r="S63" s="35">
+      <c r="S68" s="35">
         <v>62625</v>
       </c>
-      <c r="T63" s="35">
+      <c r="T68" s="35">
         <v>57816</v>
       </c>
-      <c r="U63" s="35">
+      <c r="U68" s="35">
         <v>56977</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P64" s="35">
-        <f t="shared" ref="P64:Q64" si="26">P63+P61</f>
+      <c r="P69" s="35">
+        <f t="shared" ref="P69:Q69" si="34">P68+P66</f>
         <v>142890</v>
       </c>
-      <c r="Q64" s="35">
-        <f t="shared" si="26"/>
+      <c r="Q69" s="35">
+        <f t="shared" si="34"/>
         <v>134612</v>
       </c>
-      <c r="R64" s="35">
-        <f>R63+R61</f>
+      <c r="R69" s="35">
+        <f>R68+R66</f>
         <v>142862</v>
       </c>
-      <c r="S64" s="35">
-        <f>S63+S61</f>
+      <c r="S69" s="35">
+        <f>S68+S66</f>
         <v>167117</v>
       </c>
-      <c r="T64" s="35">
-        <f>T63+T61</f>
+      <c r="T69" s="35">
+        <f>T68+T66</f>
         <v>155063</v>
       </c>
-      <c r="U64" s="35">
-        <f>U63+U61</f>
+      <c r="U69" s="35">
+        <f>U68+U66</f>
         <v>153953</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="P66" s="35">
-        <f t="shared" ref="P66:R66" si="27">P48-P61</f>
+      <c r="P71" s="35">
+        <f t="shared" ref="P71:R71" si="35">P53-P66</f>
         <v>85513</v>
       </c>
-      <c r="Q66" s="35">
-        <f t="shared" si="27"/>
+      <c r="Q71" s="35">
+        <f t="shared" si="35"/>
         <v>79606</v>
       </c>
-      <c r="R66" s="35">
-        <f t="shared" si="27"/>
+      <c r="R71" s="35">
+        <f t="shared" si="35"/>
         <v>63445</v>
       </c>
-      <c r="S66" s="35">
-        <f t="shared" ref="S66" si="28">S48-S61</f>
+      <c r="S71" s="35">
+        <f t="shared" ref="S71" si="36">S53-S66</f>
         <v>63676</v>
       </c>
-      <c r="T66" s="35">
-        <f>T48-T61</f>
+      <c r="T71" s="35">
+        <f>T53-T66</f>
         <v>57816</v>
       </c>
-      <c r="U66" s="35">
-        <f>U48-U61</f>
+      <c r="U71" s="35">
+        <f>U53-U66</f>
         <v>56977</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P67" s="1">
-        <f t="shared" ref="P67:R67" si="29">P66/P21</f>
+      <c r="P72" s="1">
+        <f t="shared" ref="P72:R72" si="37">P71/P26</f>
         <v>3.0572021021772549</v>
       </c>
-      <c r="Q67" s="1">
-        <f t="shared" si="29"/>
+      <c r="Q72" s="1">
+        <f t="shared" si="37"/>
         <v>2.8666186532229023</v>
       </c>
-      <c r="R67" s="1">
-        <f t="shared" si="29"/>
+      <c r="R72" s="1">
+        <f t="shared" si="37"/>
         <v>2.2981490201760422</v>
       </c>
-      <c r="S67" s="1">
-        <f t="shared" ref="S67" si="30">S66/S21</f>
+      <c r="S72" s="1">
+        <f t="shared" ref="S72" si="38">S71/S26</f>
         <v>2.1627606820188845</v>
       </c>
-      <c r="T67" s="1">
-        <f>T66/T21</f>
+      <c r="T72" s="1">
+        <f>T71/T26</f>
         <v>1.9537712895377128</v>
       </c>
-      <c r="U67" s="1">
-        <f>U66/U21</f>
+      <c r="U72" s="1">
+        <f>U71/U26</f>
         <v>1.9639114849027988</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B69" s="1" t="s">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Q69" s="38">
-        <f t="shared" ref="Q69" si="31">Q42/P42-1</f>
+      <c r="Q74" s="38">
+        <f t="shared" ref="Q74" si="39">Q47/P47-1</f>
         <v>8.6805555555555802E-3</v>
       </c>
-      <c r="R69" s="38">
-        <f t="shared" ref="R69" si="32">R42/Q42-1</f>
+      <c r="R74" s="38">
+        <f t="shared" ref="R74" si="40">R47/Q47-1</f>
         <v>0.22891566265060237</v>
       </c>
-      <c r="S69" s="38">
-        <f t="shared" ref="S69:T69" si="33">S42/R42-1</f>
+      <c r="S74" s="38">
+        <f t="shared" ref="S74:T74" si="41">S47/R47-1</f>
         <v>-0.18067226890756305</v>
       </c>
-      <c r="T69" s="38">
-        <f t="shared" si="33"/>
+      <c r="T74" s="38">
+        <f t="shared" si="41"/>
         <v>0.15555555555555545</v>
       </c>
-      <c r="U69" s="38">
-        <f>U42/T42-1</f>
+      <c r="U74" s="38">
+        <f>U47/T47-1</f>
         <v>0.23668639053254448</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B70" s="1" t="s">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="40" t="s">
+    <row r="77" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="41"/>
-      <c r="F72" s="41"/>
-      <c r="H72" s="41"/>
-      <c r="J72" s="41"/>
-      <c r="L72" s="41"/>
-      <c r="P72" s="42">
-        <f t="shared" ref="P72:R72" si="34">P46</f>
+      <c r="D77" s="41"/>
+      <c r="F77" s="41"/>
+      <c r="H77" s="41"/>
+      <c r="J77" s="41"/>
+      <c r="L77" s="41"/>
+      <c r="P77" s="42">
+        <f t="shared" ref="P77:R77" si="42">P51</f>
         <v>8835</v>
       </c>
-      <c r="Q72" s="42">
-        <f t="shared" si="34"/>
+      <c r="Q77" s="42">
+        <f t="shared" si="42"/>
         <v>4674</v>
       </c>
-      <c r="R72" s="42">
-        <f t="shared" si="34"/>
+      <c r="R77" s="42">
+        <f t="shared" si="42"/>
         <v>13637</v>
       </c>
-      <c r="S72" s="42">
-        <f t="shared" ref="S72" si="35">S46</f>
+      <c r="S77" s="42">
+        <f t="shared" ref="S77" si="43">S51</f>
         <v>13284</v>
       </c>
-      <c r="T72" s="42">
-        <f t="shared" ref="T72" si="36">T46</f>
+      <c r="T77" s="42">
+        <f t="shared" ref="T77" si="44">T51</f>
         <v>5821</v>
       </c>
-      <c r="U72" s="42">
-        <f>U46</f>
+      <c r="U77" s="42">
+        <f>U51</f>
         <v>7496</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="40" t="s">
+      <c r="V77" s="65"/>
+    </row>
+    <row r="78" spans="1:22" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D73" s="41"/>
-      <c r="F73" s="41"/>
-      <c r="H73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="L73" s="41"/>
-      <c r="P73" s="42">
-        <f t="shared" ref="P73:R73" si="37">P50+P56+P57</f>
+      <c r="D78" s="41"/>
+      <c r="F78" s="41"/>
+      <c r="H78" s="41"/>
+      <c r="J78" s="41"/>
+      <c r="L78" s="41"/>
+      <c r="P78" s="42">
+        <f t="shared" ref="P78:R78" si="45">P55+P61+P62</f>
         <v>46574</v>
       </c>
-      <c r="Q73" s="42">
-        <f t="shared" si="37"/>
+      <c r="Q78" s="42">
+        <f t="shared" si="45"/>
         <v>43259</v>
       </c>
-      <c r="R73" s="42">
-        <f t="shared" si="37"/>
+      <c r="R78" s="42">
+        <f t="shared" si="45"/>
         <v>54799</v>
       </c>
-      <c r="S73" s="42">
-        <f t="shared" ref="S73" si="38">S50+S56+S57</f>
+      <c r="S78" s="42">
+        <f t="shared" ref="S78" si="46">S55+S61+S62</f>
         <v>76568</v>
       </c>
-      <c r="T73" s="42">
-        <f t="shared" ref="T73" si="39">T50+T56+T57</f>
+      <c r="T78" s="42">
+        <f t="shared" ref="T78" si="47">T55+T61+T62</f>
         <v>68252</v>
       </c>
-      <c r="U73" s="42">
-        <f>U50+U56+U57</f>
+      <c r="U78" s="42">
+        <f>U55+U61+U62</f>
         <v>70586</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B74" s="1" t="s">
+      <c r="V78" s="65"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P74" s="35">
-        <f t="shared" ref="P74:R74" si="40">P72-P73</f>
+      <c r="P79" s="35">
+        <f t="shared" ref="P79:R79" si="48">P77-P78</f>
         <v>-37739</v>
       </c>
-      <c r="Q74" s="35">
-        <f t="shared" si="40"/>
+      <c r="Q79" s="35">
+        <f t="shared" si="48"/>
         <v>-38585</v>
       </c>
-      <c r="R74" s="35">
-        <f t="shared" si="40"/>
+      <c r="R79" s="35">
+        <f t="shared" si="48"/>
         <v>-41162</v>
       </c>
-      <c r="S74" s="35">
-        <f t="shared" ref="S74" si="41">S72-S73</f>
+      <c r="S79" s="35">
+        <f t="shared" ref="S79" si="49">S77-S78</f>
         <v>-63284</v>
       </c>
-      <c r="T74" s="35">
-        <f t="shared" ref="T74" si="42">T72-T73</f>
+      <c r="T79" s="35">
+        <f t="shared" ref="T79" si="50">T77-T78</f>
         <v>-62431</v>
       </c>
-      <c r="U74" s="35">
-        <f>U72-U73</f>
+      <c r="U79" s="35">
+        <f>U77-U78</f>
         <v>-63090</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="43"/>
-      <c r="B75" s="44" t="s">
+    <row r="80" spans="1:22" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="43"/>
+      <c r="B80" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="D75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="H75" s="48"/>
-      <c r="J75" s="48"/>
-      <c r="L75" s="48"/>
-      <c r="P75" s="49">
-        <f t="shared" ref="P75:R75" si="43">P74*P81</f>
+      <c r="D80" s="48"/>
+      <c r="F80" s="48"/>
+      <c r="H80" s="48"/>
+      <c r="J80" s="48"/>
+      <c r="L80" s="48"/>
+      <c r="P80" s="49">
+        <f t="shared" ref="P80:R80" si="51">P79*P86</f>
         <v>-32323.453500000003</v>
       </c>
-      <c r="Q75" s="49">
-        <f t="shared" si="43"/>
+      <c r="Q80" s="49">
+        <f t="shared" si="51"/>
         <v>-33835.186500000003</v>
       </c>
-      <c r="R75" s="49">
-        <f t="shared" si="43"/>
+      <c r="R80" s="49">
+        <f t="shared" si="51"/>
         <v>-35407.5524</v>
       </c>
-      <c r="S75" s="49">
-        <f t="shared" ref="S75" si="44">S74*S81</f>
+      <c r="S80" s="49">
+        <f t="shared" ref="S80" si="52">S79*S86</f>
         <v>-56411.357599999996</v>
       </c>
-      <c r="T75" s="49">
-        <f t="shared" ref="T75" si="45">T74*T81</f>
+      <c r="T80" s="49">
+        <f t="shared" ref="T80" si="53">T79*T86</f>
         <v>-53241.156799999997</v>
       </c>
-      <c r="U75" s="49">
-        <f>U74*U81</f>
+      <c r="U80" s="49">
+        <f>U79*U86</f>
         <v>-53582.337000000007</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
+      <c r="V80" s="70"/>
+    </row>
+    <row r="82" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B82" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="P77" s="1">
+      <c r="P82" s="1">
         <v>2.081</v>
       </c>
-      <c r="Q77" s="1">
+      <c r="Q82" s="1">
         <v>1.9421999999999999</v>
       </c>
-      <c r="R77" s="1">
+      <c r="R82" s="1">
         <v>1.1020000000000001</v>
       </c>
-      <c r="S77" s="1">
+      <c r="S82" s="1">
         <v>1.1434</v>
       </c>
-      <c r="T77" s="1">
+      <c r="T82" s="1">
         <v>1.3188</v>
       </c>
-      <c r="U77" s="1">
+      <c r="U82" s="1">
         <v>1.2484</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B78" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P78" s="50">
-        <f t="shared" ref="P78:R78" si="46">P77*P21</f>
-        <v>58207.650999999998</v>
-      </c>
-      <c r="Q78" s="50">
-        <f t="shared" si="46"/>
-        <v>53934.894</v>
-      </c>
-      <c r="R78" s="50">
-        <f t="shared" si="46"/>
-        <v>30422.914000000004</v>
-      </c>
-      <c r="S78" s="50">
-        <f t="shared" ref="S78" si="47">S77*S21</f>
-        <v>33663.982799999998</v>
-      </c>
-      <c r="T78" s="50">
-        <f t="shared" ref="T78" si="48">T77*T21</f>
-        <v>39025.929599999996</v>
-      </c>
-      <c r="U78" s="50">
-        <f>U77*U21</f>
-        <v>36218.580799999996</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B79" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P79" s="50">
-        <f t="shared" ref="P79:R79" si="49">P78-P75</f>
-        <v>90531.104500000001</v>
-      </c>
-      <c r="Q79" s="50">
-        <f t="shared" si="49"/>
-        <v>87770.080500000011</v>
-      </c>
-      <c r="R79" s="50">
-        <f t="shared" si="49"/>
-        <v>65830.466400000005</v>
-      </c>
-      <c r="S79" s="50">
-        <f t="shared" ref="S79" si="50">S78-S75</f>
-        <v>90075.340399999986</v>
-      </c>
-      <c r="T79" s="50">
-        <f t="shared" ref="T79" si="51">T78-T75</f>
-        <v>92267.0864</v>
-      </c>
-      <c r="U79" s="50">
-        <f>U78-U75</f>
-        <v>89800.917799999996</v>
-      </c>
-    </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B81" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="P81" s="1">
-        <v>0.85650000000000004</v>
-      </c>
-      <c r="Q81" s="1">
-        <v>0.87690000000000001</v>
-      </c>
-      <c r="R81" s="1">
-        <v>0.86019999999999996</v>
-      </c>
-      <c r="S81" s="1">
-        <v>0.89139999999999997</v>
-      </c>
-      <c r="T81" s="1">
-        <v>0.8528</v>
-      </c>
-      <c r="U81" s="1">
-        <v>0.84930000000000005</v>
       </c>
     </row>
     <row r="83" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P83" s="50">
+        <f t="shared" ref="P83:R83" si="54">P82*P26</f>
+        <v>58207.650999999998</v>
+      </c>
+      <c r="Q83" s="50">
+        <f t="shared" si="54"/>
+        <v>53934.894</v>
+      </c>
+      <c r="R83" s="50">
+        <f t="shared" si="54"/>
+        <v>30422.914000000004</v>
+      </c>
+      <c r="S83" s="50">
+        <f t="shared" ref="S83" si="55">S82*S26</f>
+        <v>33663.982799999998</v>
+      </c>
+      <c r="T83" s="50">
+        <f t="shared" ref="T83" si="56">T82*T26</f>
+        <v>39025.929599999996</v>
+      </c>
+      <c r="U83" s="50">
+        <f>U82*U26</f>
+        <v>36218.580799999996</v>
+      </c>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P84" s="50">
+        <f t="shared" ref="P84:R84" si="57">P83-P80</f>
+        <v>90531.104500000001</v>
+      </c>
+      <c r="Q84" s="50">
+        <f t="shared" si="57"/>
+        <v>87770.080500000011</v>
+      </c>
+      <c r="R84" s="50">
+        <f t="shared" si="57"/>
+        <v>65830.466400000005</v>
+      </c>
+      <c r="S84" s="50">
+        <f t="shared" ref="S84" si="58">S83-S80</f>
+        <v>90075.340399999986</v>
+      </c>
+      <c r="T84" s="50">
+        <f t="shared" ref="T84" si="59">T83-T80</f>
+        <v>92267.0864</v>
+      </c>
+      <c r="U84" s="50">
+        <f>U83-U80</f>
+        <v>89800.917799999996</v>
+      </c>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B86" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P86" s="1">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>0.87690000000000001</v>
+      </c>
+      <c r="R86" s="1">
+        <v>0.86019999999999996</v>
+      </c>
+      <c r="S86" s="1">
+        <v>0.89139999999999997</v>
+      </c>
+      <c r="T86" s="1">
+        <v>0.8528</v>
+      </c>
+      <c r="U86" s="1">
+        <v>0.84930000000000005</v>
+      </c>
+    </row>
+    <row r="88" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B88" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P83" s="52">
-        <f t="shared" ref="P83:R83" si="52">P77/P67</f>
+      <c r="P88" s="52">
+        <f t="shared" ref="P88:Q88" si="60">P82/P72</f>
         <v>0.68068774338404692</v>
       </c>
-      <c r="Q83" s="52">
-        <f t="shared" si="52"/>
+      <c r="Q88" s="52">
+        <f t="shared" si="60"/>
         <v>0.67752297565510133</v>
       </c>
-      <c r="R83" s="52">
-        <f t="shared" ref="R83:T83" si="53">R77/R67</f>
+      <c r="R88" s="52">
+        <f t="shared" ref="R88:T88" si="61">R82/R72</f>
         <v>0.47951633698479007</v>
       </c>
-      <c r="S83" s="52">
-        <f t="shared" si="53"/>
+      <c r="S88" s="52">
+        <f t="shared" si="61"/>
         <v>0.52867615428104786</v>
       </c>
-      <c r="T83" s="52">
-        <f t="shared" si="53"/>
+      <c r="T88" s="52">
+        <f t="shared" si="61"/>
         <v>0.67500224159402245</v>
       </c>
-      <c r="U83" s="52">
-        <f>U77/U67</f>
+      <c r="U88" s="52">
+        <f>U82/U72</f>
         <v>0.6356701967460554</v>
       </c>
     </row>
-    <row r="85" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B85" s="1" t="s">
+    <row r="90" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B90" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P85" s="52">
-        <f t="shared" ref="P85:R85" si="54">P77/P20</f>
+      <c r="P90" s="52">
+        <f t="shared" ref="P90:Q90" si="62">P82/P25</f>
         <v>-29.517064401622715</v>
       </c>
-      <c r="Q85" s="52">
-        <f t="shared" si="54"/>
+      <c r="Q90" s="52">
+        <f t="shared" si="62"/>
         <v>11.338005886062644</v>
       </c>
-      <c r="R85" s="52">
-        <f t="shared" ref="R85:T85" si="55">R77/R20</f>
+      <c r="R90" s="52">
+        <f t="shared" ref="R90:T90" si="63">R82/R25</f>
         <v>-7.4039703090776356</v>
       </c>
-      <c r="S85" s="52">
-        <f t="shared" si="55"/>
+      <c r="S90" s="52">
+        <f t="shared" si="63"/>
         <v>-73.986775384615385</v>
       </c>
-      <c r="T85" s="52">
-        <f t="shared" si="55"/>
+      <c r="T90" s="52">
+        <f t="shared" si="63"/>
         <v>72.80957014925373</v>
       </c>
-      <c r="U85" s="52">
-        <f>U77/U20</f>
+      <c r="U90" s="52">
+        <f>U82/U25</f>
         <v>13.802812804878048</v>
       </c>
     </row>

</xml_diff>